<commit_message>
feature: topic 3 added
</commit_message>
<xml_diff>
--- a/public/innovation_marketing_questions.xlsx
+++ b/public/innovation_marketing_questions.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrykostern/Documents/code/innovation-mgt/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08315F30-CE72-E644-86FE-0E2DA35AED99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6B0F3B-5A25-ED4B-98A3-2A33EA18A5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principles of Marketing &amp; Ethic" sheetId="1" r:id="rId1"/>
     <sheet name="Marketing Strategy and Environm" sheetId="2" r:id="rId2"/>
+    <sheet name="Creating Customer Value, Satisf" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="681">
   <si>
     <t>Question</t>
   </si>
@@ -1368,15 +1369,719 @@
   </si>
   <si>
     <t>Cusomer relationships</t>
+  </si>
+  <si>
+    <t>Which of the following best captures the conceptual definition of customer-perceived value?</t>
+  </si>
+  <si>
+    <t>The sum of all benefits a customer receives from a product, regardless of cost</t>
+  </si>
+  <si>
+    <t>The difference between a customer’s evaluation of benefits and costs relative to alternatives</t>
+  </si>
+  <si>
+    <t>The total costs incurred by a customer when purchasing and using a product</t>
+  </si>
+  <si>
+    <t>The emotional bond formed through high customer satisfaction</t>
+  </si>
+  <si>
+    <t>Customer-perceived value is defined as the benefit–cost tradeoff a customer perceives compared to alternatives.</t>
+  </si>
+  <si>
+    <t>Which is not one of the four steps in conducting a customer-perceived value analysis?</t>
+  </si>
+  <si>
+    <t>Identifying major benefits and costs from the customer’s perspective</t>
+  </si>
+  <si>
+    <t>Assessing competitor performance against importance weights</t>
+  </si>
+  <si>
+    <t>Estimating the net present value of future customer profits</t>
+  </si>
+  <si>
+    <t>Monitoring performance over time for both company and competitors</t>
+  </si>
+  <si>
+    <t>Value analysis focuses on customer benefits and costs, not on company profit calculations.</t>
+  </si>
+  <si>
+    <t>In the confirmation/disconfirmation paradigm, what outcome corresponds to P &gt; E?</t>
+  </si>
+  <si>
+    <t>Negative disconfirmation</t>
+  </si>
+  <si>
+    <t>Confirmation</t>
+  </si>
+  <si>
+    <t>Positive disconfirmation</t>
+  </si>
+  <si>
+    <t>Cognitive dissonance</t>
+  </si>
+  <si>
+    <t>When perceived performance (P) exceeds expectations (E), positive disconfirmation occurs.</t>
+  </si>
+  <si>
+    <t>Which factor does not directly shape buyers’ pre-purchase expectations (E)?</t>
+  </si>
+  <si>
+    <t>Past buying experience</t>
+  </si>
+  <si>
+    <t>Friends’ and associates’ advice</t>
+  </si>
+  <si>
+    <t>Marketing promises</t>
+  </si>
+  <si>
+    <t>Current product usage costs</t>
+  </si>
+  <si>
+    <t>Usage costs affect perceived value but do not form pre-purchase expectations.</t>
+  </si>
+  <si>
+    <t>“Delight” in the context of customer satisfaction refers to:</t>
+  </si>
+  <si>
+    <t>Satisfaction exactly matching expectations</t>
+  </si>
+  <si>
+    <t>Very low satisfaction leading to churn</t>
+  </si>
+  <si>
+    <t>Very high satisfaction creating an emotional bond</t>
+  </si>
+  <si>
+    <t>Indifference to competitor offerings</t>
+  </si>
+  <si>
+    <t>Delight occurs when performance greatly exceeds expectations, creating strong emotional bonds.</t>
+  </si>
+  <si>
+    <t>Which is not a reason why satisfied customers are valuable?</t>
+  </si>
+  <si>
+    <t>They cost less to serve than new customers</t>
+  </si>
+  <si>
+    <t>They have lower sensitivity to price</t>
+  </si>
+  <si>
+    <t>They rarely participate in word-of-mouth promotion</t>
+  </si>
+  <si>
+    <t>They are more likely to buy new offerings</t>
+  </si>
+  <si>
+    <t>Satisfied customers often promote via word-of-mouth, so rarity of such promotion is not a value point.</t>
+  </si>
+  <si>
+    <t>A main challenge in acting on patient satisfaction surveys is:</t>
+  </si>
+  <si>
+    <t>Ensuring high switching costs</t>
+  </si>
+  <si>
+    <t>Balancing ethical and financial metrics</t>
+  </si>
+  <si>
+    <t>Obtaining valid and reliable data across services</t>
+  </si>
+  <si>
+    <t>Maximizing customer equity directly</t>
+  </si>
+  <si>
+    <t>Collecting consistent data across varied services is a key challenge for validity and reliability.</t>
+  </si>
+  <si>
+    <t>Which is not an effective response to customer dissatisfaction?</t>
+  </si>
+  <si>
+    <t>Accept responsibility for the disappointment</t>
+  </si>
+  <si>
+    <t>Delay contacting the customer to investigate fully</t>
+  </si>
+  <si>
+    <t>Use empathetic service personnel</t>
+  </si>
+  <si>
+    <t>Resolve complaints quickly</t>
+  </si>
+  <si>
+    <t>Delaying contact frustrates customers; prompt response is crucial.</t>
+  </si>
+  <si>
+    <t>Customer loyalty is best defined as:</t>
+  </si>
+  <si>
+    <t>Immediate repeat purchase</t>
+  </si>
+  <si>
+    <t>Deeply held commitment to re-buy despite switching influences</t>
+  </si>
+  <si>
+    <t>High willingness to pay</t>
+  </si>
+  <si>
+    <t>Emotional satisfaction only</t>
+  </si>
+  <si>
+    <t>True loyalty involves a commitment that endures against competitive offers.</t>
+  </si>
+  <si>
+    <t>Which factor does not typically impact customer loyalty?</t>
+  </si>
+  <si>
+    <t>Contractual factors like binding agreements</t>
+  </si>
+  <si>
+    <t>Economic factors like switching costs</t>
+  </si>
+  <si>
+    <t>Color of product packaging</t>
+  </si>
+  <si>
+    <t>Situational factors like store proximity</t>
+  </si>
+  <si>
+    <t>Packaging color is not a systematic driver of loyalty.</t>
+  </si>
+  <si>
+    <t>A company with a highly loyal customer base will likely experience:</t>
+  </si>
+  <si>
+    <t>Higher acquisition costs over time</t>
+  </si>
+  <si>
+    <t>Lower sensitivity to competitive offers</t>
+  </si>
+  <si>
+    <t>Reduced product usage</t>
+  </si>
+  <si>
+    <t>Increased price elasticity</t>
+  </si>
+  <si>
+    <t>Loyal customers are less likely to switch when competitors offer alternatives.</t>
+  </si>
+  <si>
+    <t>Which dimension of customer engagement describes whether the impact is positive or negative?</t>
+  </si>
+  <si>
+    <t>Nature of impact</t>
+  </si>
+  <si>
+    <t>Modality</t>
+  </si>
+  <si>
+    <t>Valence</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>Valence indicates the positivity or negativity of engagement.</t>
+  </si>
+  <si>
+    <t>“Modality” in customer engagement refers to:</t>
+  </si>
+  <si>
+    <t>The duration of engagement</t>
+  </si>
+  <si>
+    <t>Whether engagement is in-role or extra-role</t>
+  </si>
+  <si>
+    <t>The number of different interaction channels</t>
+  </si>
+  <si>
+    <t>The immediate intensity of engagement</t>
+  </si>
+  <si>
+    <t>Modality classifies engagement as part of normal duties (in-role) or discretionary (extra-role).</t>
+  </si>
+  <si>
+    <t>An example of extra-role engagement would be:</t>
+  </si>
+  <si>
+    <t>Purchasing a new product online</t>
+  </si>
+  <si>
+    <t>Complaining via official hotline</t>
+  </si>
+  <si>
+    <t>Writing a positive online review unprompted</t>
+  </si>
+  <si>
+    <t>Using the product as intended</t>
+  </si>
+  <si>
+    <t>Writing unsolicited reviews is beyond required behaviors, thus extra-role.</t>
+  </si>
+  <si>
+    <t>Which is not one of the three primary CRM stages?</t>
+  </si>
+  <si>
+    <t>Acquisition</t>
+  </si>
+  <si>
+    <t>Abandonment</t>
+  </si>
+  <si>
+    <t>Retention</t>
+  </si>
+  <si>
+    <t>Recovery</t>
+  </si>
+  <si>
+    <t>Abandonment is not a CRM stage; CRM focuses on acquiring, retaining, and recovering customers.</t>
+  </si>
+  <si>
+    <t>CRM’s extension into customer experience management emphasizes:</t>
+  </si>
+  <si>
+    <t>Higher switching costs</t>
+  </si>
+  <si>
+    <t>Optimizing individual touchpoints and journey orientation</t>
+  </si>
+  <si>
+    <t>Focusing solely on acquisition metrics</t>
+  </si>
+  <si>
+    <t>Reducing customer survival rates</t>
+  </si>
+  <si>
+    <t>Experience management centers on the holistic customer journey and touchpoint quality.</t>
+  </si>
+  <si>
+    <t>One-to-one marketing becomes feasible when:</t>
+  </si>
+  <si>
+    <t>Aggregate market data is plentiful</t>
+  </si>
+  <si>
+    <t>Individual customer information is available</t>
+  </si>
+  <si>
+    <t>Switching costs are minimal</t>
+  </si>
+  <si>
+    <t>CLV is negative</t>
+  </si>
+  <si>
+    <t>Customized marketing requires detailed data about individual customers.</t>
+  </si>
+  <si>
+    <t>Which is not a goal of CRM?</t>
+  </si>
+  <si>
+    <t>Decreasing customer defection rate</t>
+  </si>
+  <si>
+    <t>Enhancing growth potential of each customer</t>
+  </si>
+  <si>
+    <t>Maximizing short-term profit irrespective of loyalty</t>
+  </si>
+  <si>
+    <t>Making no-profit customers more profitable or ceasing to serve them</t>
+  </si>
+  <si>
+    <t>CRM aims for profitable, loyal relationships, not just short-term profits at any cost.</t>
+  </si>
+  <si>
+    <t>Customer Lifetime Value (CLV) is calculated using:</t>
+  </si>
+  <si>
+    <t>Sum of all revenues only</t>
+  </si>
+  <si>
+    <t>Net present value of expected future profits from a customer</t>
+  </si>
+  <si>
+    <t>Current account balance of the customer</t>
+  </si>
+  <si>
+    <t>Historical purchase frequency without discounting</t>
+  </si>
+  <si>
+    <t>CLV uses discounted future profit estimates, not just raw revenues.</t>
+  </si>
+  <si>
+    <t>Discount rate per period</t>
+  </si>
+  <si>
+    <t>Hazard rate at time t</t>
+  </si>
+  <si>
+    <t>Predicted probability the customer remains active after t</t>
+  </si>
+  <si>
+    <t>Predicted profit margin per transaction</t>
+  </si>
+  <si>
+    <t>Which is not a component of customer equity?</t>
+  </si>
+  <si>
+    <t>CLV for each individual in the segment</t>
+  </si>
+  <si>
+    <t>Customer Referral Value (CRV)</t>
+  </si>
+  <si>
+    <t>Customer Influencer Value (CIV)</t>
+  </si>
+  <si>
+    <t>Price elasticity of demand</t>
+  </si>
+  <si>
+    <t>Customer equity comprises CLV, CRV, CIV, and CKV, not price elasticity.</t>
+  </si>
+  <si>
+    <t>Customer Referral Value (CRV) measures:</t>
+  </si>
+  <si>
+    <t>Direct NPS score of a customer</t>
+  </si>
+  <si>
+    <t>Net present value of customers acquired via referrals</t>
+  </si>
+  <si>
+    <t>Lifetime loyalty score</t>
+  </si>
+  <si>
+    <t>Average spending per referral</t>
+  </si>
+  <si>
+    <t>CRV quantifies the value of new customers gained through referrals.</t>
+  </si>
+  <si>
+    <t>Customer Knowledge Value (CKV) captures:</t>
+  </si>
+  <si>
+    <t>Value from open innovation contributions of customers</t>
+  </si>
+  <si>
+    <t>Educational attainment of customer base</t>
+  </si>
+  <si>
+    <t>Knowledge cost savings in production</t>
+  </si>
+  <si>
+    <t>Information asymmetry in pricing</t>
+  </si>
+  <si>
+    <t>CKV reflects the benefits from customer ideas and feedback used in innovation.</t>
+  </si>
+  <si>
+    <t>Which type of benefit is not part of the perceived‐value components?</t>
+  </si>
+  <si>
+    <t>Quality indicators</t>
+  </si>
+  <si>
+    <t>Emotional benefits</t>
+  </si>
+  <si>
+    <t>Monetary savings</t>
+  </si>
+  <si>
+    <t>Discount rate</t>
+  </si>
+  <si>
+    <t>Discount rates are financial factors in CLV, not a direct perceived benefit.</t>
+  </si>
+  <si>
+    <t>When monitoring performance over time in value analysis, a company should track:</t>
+  </si>
+  <si>
+    <t>Only its own benefit scores</t>
+  </si>
+  <si>
+    <t>Only cost metrics against industry benchmarks</t>
+  </si>
+  <si>
+    <t>Both its and competitors’ benefit and cost scores</t>
+  </si>
+  <si>
+    <t>Only qualitative customer feedback</t>
+  </si>
+  <si>
+    <t>Comparing both benefit and cost scores over time for company and competitors is key.</t>
+  </si>
+  <si>
+    <t>A negative disconfirmation occurs when:</t>
+  </si>
+  <si>
+    <t>P = E</t>
+  </si>
+  <si>
+    <t>P &lt; E</t>
+  </si>
+  <si>
+    <t>P &gt; E</t>
+  </si>
+  <si>
+    <t>P ≫ E</t>
+  </si>
+  <si>
+    <t>Negative disconfirmation is when performance falls short of expectations.</t>
+  </si>
+  <si>
+    <t>Which is a situational factor affecting loyalty?</t>
+  </si>
+  <si>
+    <t>Personal relationship with staff</t>
+  </si>
+  <si>
+    <t>Store proximity to the customer’s home</t>
+  </si>
+  <si>
+    <t>Software compatibility requirements</t>
+  </si>
+  <si>
+    <t>Contractual lock-in options</t>
+  </si>
+  <si>
+    <t>Situational factors include physical convenience like store location.</t>
+  </si>
+  <si>
+    <t>Under CRM, “interact with individual customers” primarily aims to:</t>
+  </si>
+  <si>
+    <t>Aggregate purchase data only</t>
+  </si>
+  <si>
+    <t>Customize communications and offers</t>
+  </si>
+  <si>
+    <t>Increase switching costs</t>
+  </si>
+  <si>
+    <t>Standardize product features</t>
+  </si>
+  <si>
+    <t>The goal is personalized interactions tailored to each customer's needs.</t>
+  </si>
+  <si>
+    <t>Which describes “scope” in engagement dimensions?</t>
+  </si>
+  <si>
+    <t>Positive versus negative impact</t>
+  </si>
+  <si>
+    <t>Geographic and temporal reach of engagement</t>
+  </si>
+  <si>
+    <t>Intensity of resource investment</t>
+  </si>
+  <si>
+    <t>In-role versus extra-role behaviors</t>
+  </si>
+  <si>
+    <t>Scope refers to how broadly engagement is spread over time and space.</t>
+  </si>
+  <si>
+    <t>A high “breadth” in engagement nature indicates:</t>
+  </si>
+  <si>
+    <t>Engagement across many channels or activities</t>
+  </si>
+  <si>
+    <t>Single, intense interaction moment</t>
+  </si>
+  <si>
+    <t>Predominantly negative valence</t>
+  </si>
+  <si>
+    <t>Short-lived interaction only</t>
+  </si>
+  <si>
+    <t>Breadth refers to the variety of channels or activities in which engagement occurs.</t>
+  </si>
+  <si>
+    <t>Which economic factor can enhance loyalty?</t>
+  </si>
+  <si>
+    <t>Low switching costs</t>
+  </si>
+  <si>
+    <t>High switching costs</t>
+  </si>
+  <si>
+    <t>Zero contractual obligations</t>
+  </si>
+  <si>
+    <t>High switching costs create a financial barrier to switching away.</t>
+  </si>
+  <si>
+    <t>In CLV calculations, a higher discount rate (i) will:</t>
+  </si>
+  <si>
+    <t>Increase CLV</t>
+  </si>
+  <si>
+    <t>Have no effect on CLV</t>
+  </si>
+  <si>
+    <t>Decrease CLV</t>
+  </si>
+  <si>
+    <t>Only affect CRV</t>
+  </si>
+  <si>
+    <t>A higher discount rate reduces the present value of future profits.</t>
+  </si>
+  <si>
+    <t>The primary goal of customer recovery in CRM is to:</t>
+  </si>
+  <si>
+    <t>Acquire new customers cost-effectively</t>
+  </si>
+  <si>
+    <t>Restore relationships with lost or defecting customers</t>
+  </si>
+  <si>
+    <t>Increase survival rate beyond 1 period</t>
+  </si>
+  <si>
+    <t>Maximize short-term profit per transaction</t>
+  </si>
+  <si>
+    <t>Recovery focuses on winning back customers who have defected.</t>
+  </si>
+  <si>
+    <t>Which is not a marketing outcome of high customer satisfaction?</t>
+  </si>
+  <si>
+    <t>Increased word-of-mouth promotion</t>
+  </si>
+  <si>
+    <t>Reduced attention to competing brands</t>
+  </si>
+  <si>
+    <t>Higher sensitivity to price increases</t>
+  </si>
+  <si>
+    <t>Longer relationship duration</t>
+  </si>
+  <si>
+    <t>Satisfied customers are less sensitive to price, not more.</t>
+  </si>
+  <si>
+    <t>A tactical focus on optimizing service touchpoints is part of:</t>
+  </si>
+  <si>
+    <t>Customer-perceived value analysis</t>
+  </si>
+  <si>
+    <t>Customer experience management</t>
+  </si>
+  <si>
+    <t>CLV calculation</t>
+  </si>
+  <si>
+    <t>Referral value analysis</t>
+  </si>
+  <si>
+    <t>Experience management emphasizes touchpoint-level optimizations.</t>
+  </si>
+  <si>
+    <t>Which loyalty driver is psychological rather than economic?</t>
+  </si>
+  <si>
+    <t>Contract term length</t>
+  </si>
+  <si>
+    <t>Personal relations with staff</t>
+  </si>
+  <si>
+    <t>Software lock-in</t>
+  </si>
+  <si>
+    <t>Switching fees</t>
+  </si>
+  <si>
+    <t>Personal relationships tap into emotional bonds, a psychological driver.</t>
+  </si>
+  <si>
+    <t>Customer Influencer Value (CIV) quantifies:</t>
+  </si>
+  <si>
+    <t>Value from customers’ own referrals only</t>
+  </si>
+  <si>
+    <t>Value from customers influencing others via reviews, leadership</t>
+  </si>
+  <si>
+    <t>Cost savings from customer service automation</t>
+  </si>
+  <si>
+    <t>Knowledge contributions to R&amp;D</t>
+  </si>
+  <si>
+    <t>CIV measures the impact of customers influencing others beyond direct referrals.</t>
+  </si>
+  <si>
+    <t>Which cost component is considered in perceived value?</t>
+  </si>
+  <si>
+    <t>Opportunity costs</t>
+  </si>
+  <si>
+    <t>Referral incentives</t>
+  </si>
+  <si>
+    <t>Customer equity</t>
+  </si>
+  <si>
+    <t>Opportunity cost is the value of the next best alternative forgone, included in perceived costs.</t>
+  </si>
+  <si>
+    <t>To ensure survey validity and reliability, one should:</t>
+  </si>
+  <si>
+    <t>Use only open-ended questions</t>
+  </si>
+  <si>
+    <t>Employ standardized scales and pre-testing</t>
+  </si>
+  <si>
+    <t>Avoid mystery shopping</t>
+  </si>
+  <si>
+    <t>Only sample highly satisfied customers</t>
+  </si>
+  <si>
+    <t>Standardized measurement and pilot testing bolster both validity and reliability.</t>
+  </si>
+  <si>
+    <t>In the CLV formula, the term $p_{j,t}$ represents:</t>
+  </si>
+  <si>
+    <t>$p_{j,t}$ is the survival probability that the customer stays beyond period t.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1391,7 +2096,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1399,14 +2104,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2687,7 +3410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -3646,4 +4369,942 @@
     <ignoredError sqref="A2:G6 A1:F1 A8:G9 A7:E7 G7 A11:G11 A10:E10 G10 A13:G13 A12:E12 G12 A17:G17 A14:E14 G14 A15:E15 G15 A16:E16 G16 A19:G19 A18:E18 G18 A22:G23 A20:E20 G20 A21:E21 G21 A24:G24 A30:G31 A25:E25 G25 A26:E26 G26 A27:E27 G27 A28:E28 G28 A29:E29 G29 A33:G34 A32:E32 G32 A36:G36 A35:E35 G35 A37:E37 G37 A38:D38 F38:G38 A39:E39 G39 A40:E40 G40 A41:B41 D41:G41" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0184A555-D137-5947-81F3-BEB4CF021670}">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="82.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B2" t="s">
+        <v>563</v>
+      </c>
+      <c r="C2" t="s">
+        <v>564</v>
+      </c>
+      <c r="D2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>449</v>
+      </c>
+      <c r="B3" t="s">
+        <v>450</v>
+      </c>
+      <c r="C3" t="s">
+        <v>451</v>
+      </c>
+      <c r="D3" t="s">
+        <v>452</v>
+      </c>
+      <c r="E3" t="s">
+        <v>453</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>455</v>
+      </c>
+      <c r="B4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C4" t="s">
+        <v>457</v>
+      </c>
+      <c r="D4" t="s">
+        <v>458</v>
+      </c>
+      <c r="E4" t="s">
+        <v>459</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>461</v>
+      </c>
+      <c r="B5" t="s">
+        <v>462</v>
+      </c>
+      <c r="C5" t="s">
+        <v>463</v>
+      </c>
+      <c r="D5" t="s">
+        <v>464</v>
+      </c>
+      <c r="E5" t="s">
+        <v>465</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>467</v>
+      </c>
+      <c r="B6" t="s">
+        <v>468</v>
+      </c>
+      <c r="C6" t="s">
+        <v>469</v>
+      </c>
+      <c r="D6" t="s">
+        <v>470</v>
+      </c>
+      <c r="E6" t="s">
+        <v>471</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>473</v>
+      </c>
+      <c r="B7" t="s">
+        <v>474</v>
+      </c>
+      <c r="C7" t="s">
+        <v>475</v>
+      </c>
+      <c r="D7" t="s">
+        <v>476</v>
+      </c>
+      <c r="E7" t="s">
+        <v>477</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>479</v>
+      </c>
+      <c r="B8" t="s">
+        <v>480</v>
+      </c>
+      <c r="C8" t="s">
+        <v>481</v>
+      </c>
+      <c r="D8" t="s">
+        <v>482</v>
+      </c>
+      <c r="E8" t="s">
+        <v>483</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>485</v>
+      </c>
+      <c r="B9" t="s">
+        <v>486</v>
+      </c>
+      <c r="C9" t="s">
+        <v>487</v>
+      </c>
+      <c r="D9" t="s">
+        <v>488</v>
+      </c>
+      <c r="E9" t="s">
+        <v>489</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>491</v>
+      </c>
+      <c r="B10" t="s">
+        <v>492</v>
+      </c>
+      <c r="C10" t="s">
+        <v>493</v>
+      </c>
+      <c r="D10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E10" t="s">
+        <v>495</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>497</v>
+      </c>
+      <c r="B11" t="s">
+        <v>498</v>
+      </c>
+      <c r="C11" t="s">
+        <v>499</v>
+      </c>
+      <c r="D11" t="s">
+        <v>500</v>
+      </c>
+      <c r="E11" t="s">
+        <v>501</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>503</v>
+      </c>
+      <c r="B12" t="s">
+        <v>504</v>
+      </c>
+      <c r="C12" t="s">
+        <v>505</v>
+      </c>
+      <c r="D12" t="s">
+        <v>506</v>
+      </c>
+      <c r="E12" t="s">
+        <v>507</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>509</v>
+      </c>
+      <c r="B13" t="s">
+        <v>510</v>
+      </c>
+      <c r="C13" t="s">
+        <v>511</v>
+      </c>
+      <c r="D13" t="s">
+        <v>512</v>
+      </c>
+      <c r="E13" t="s">
+        <v>513</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>515</v>
+      </c>
+      <c r="B14" t="s">
+        <v>516</v>
+      </c>
+      <c r="C14" t="s">
+        <v>517</v>
+      </c>
+      <c r="D14" t="s">
+        <v>518</v>
+      </c>
+      <c r="E14" t="s">
+        <v>519</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>521</v>
+      </c>
+      <c r="B15" t="s">
+        <v>522</v>
+      </c>
+      <c r="C15" t="s">
+        <v>523</v>
+      </c>
+      <c r="D15" t="s">
+        <v>524</v>
+      </c>
+      <c r="E15" t="s">
+        <v>525</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>527</v>
+      </c>
+      <c r="B16" t="s">
+        <v>528</v>
+      </c>
+      <c r="C16" t="s">
+        <v>529</v>
+      </c>
+      <c r="D16" t="s">
+        <v>530</v>
+      </c>
+      <c r="E16" t="s">
+        <v>531</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>533</v>
+      </c>
+      <c r="B17" t="s">
+        <v>534</v>
+      </c>
+      <c r="C17" t="s">
+        <v>535</v>
+      </c>
+      <c r="D17" t="s">
+        <v>536</v>
+      </c>
+      <c r="E17" t="s">
+        <v>537</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>539</v>
+      </c>
+      <c r="B18" t="s">
+        <v>540</v>
+      </c>
+      <c r="C18" t="s">
+        <v>541</v>
+      </c>
+      <c r="D18" t="s">
+        <v>542</v>
+      </c>
+      <c r="E18" t="s">
+        <v>543</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>545</v>
+      </c>
+      <c r="B19" t="s">
+        <v>546</v>
+      </c>
+      <c r="C19" t="s">
+        <v>547</v>
+      </c>
+      <c r="D19" t="s">
+        <v>548</v>
+      </c>
+      <c r="E19" t="s">
+        <v>549</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>551</v>
+      </c>
+      <c r="B20" t="s">
+        <v>552</v>
+      </c>
+      <c r="C20" t="s">
+        <v>553</v>
+      </c>
+      <c r="D20" t="s">
+        <v>554</v>
+      </c>
+      <c r="E20" t="s">
+        <v>555</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>557</v>
+      </c>
+      <c r="B21" t="s">
+        <v>558</v>
+      </c>
+      <c r="C21" t="s">
+        <v>559</v>
+      </c>
+      <c r="D21" t="s">
+        <v>560</v>
+      </c>
+      <c r="E21" t="s">
+        <v>561</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>567</v>
+      </c>
+      <c r="B22" t="s">
+        <v>568</v>
+      </c>
+      <c r="C22" t="s">
+        <v>569</v>
+      </c>
+      <c r="D22" t="s">
+        <v>570</v>
+      </c>
+      <c r="E22" t="s">
+        <v>571</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>573</v>
+      </c>
+      <c r="B23" t="s">
+        <v>574</v>
+      </c>
+      <c r="C23" t="s">
+        <v>575</v>
+      </c>
+      <c r="D23" t="s">
+        <v>576</v>
+      </c>
+      <c r="E23" t="s">
+        <v>577</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>579</v>
+      </c>
+      <c r="B24" t="s">
+        <v>580</v>
+      </c>
+      <c r="C24" t="s">
+        <v>581</v>
+      </c>
+      <c r="D24" t="s">
+        <v>582</v>
+      </c>
+      <c r="E24" t="s">
+        <v>583</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>585</v>
+      </c>
+      <c r="B25" t="s">
+        <v>586</v>
+      </c>
+      <c r="C25" t="s">
+        <v>587</v>
+      </c>
+      <c r="D25" t="s">
+        <v>588</v>
+      </c>
+      <c r="E25" t="s">
+        <v>589</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>591</v>
+      </c>
+      <c r="B26" t="s">
+        <v>592</v>
+      </c>
+      <c r="C26" t="s">
+        <v>593</v>
+      </c>
+      <c r="D26" t="s">
+        <v>594</v>
+      </c>
+      <c r="E26" t="s">
+        <v>595</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>597</v>
+      </c>
+      <c r="B27" t="s">
+        <v>598</v>
+      </c>
+      <c r="C27" t="s">
+        <v>599</v>
+      </c>
+      <c r="D27" t="s">
+        <v>600</v>
+      </c>
+      <c r="E27" t="s">
+        <v>601</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>603</v>
+      </c>
+      <c r="B28" t="s">
+        <v>604</v>
+      </c>
+      <c r="C28" t="s">
+        <v>605</v>
+      </c>
+      <c r="D28" t="s">
+        <v>606</v>
+      </c>
+      <c r="E28" t="s">
+        <v>607</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>609</v>
+      </c>
+      <c r="B29" t="s">
+        <v>610</v>
+      </c>
+      <c r="C29" t="s">
+        <v>611</v>
+      </c>
+      <c r="D29" t="s">
+        <v>612</v>
+      </c>
+      <c r="E29" t="s">
+        <v>613</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>615</v>
+      </c>
+      <c r="B30" t="s">
+        <v>616</v>
+      </c>
+      <c r="C30" t="s">
+        <v>617</v>
+      </c>
+      <c r="D30" t="s">
+        <v>618</v>
+      </c>
+      <c r="E30" t="s">
+        <v>619</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>621</v>
+      </c>
+      <c r="B31" t="s">
+        <v>622</v>
+      </c>
+      <c r="C31" t="s">
+        <v>623</v>
+      </c>
+      <c r="D31" t="s">
+        <v>624</v>
+      </c>
+      <c r="E31" t="s">
+        <v>625</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>627</v>
+      </c>
+      <c r="B32" t="s">
+        <v>628</v>
+      </c>
+      <c r="C32" t="s">
+        <v>629</v>
+      </c>
+      <c r="D32" t="s">
+        <v>630</v>
+      </c>
+      <c r="E32" t="s">
+        <v>462</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>632</v>
+      </c>
+      <c r="B33" t="s">
+        <v>633</v>
+      </c>
+      <c r="C33" t="s">
+        <v>634</v>
+      </c>
+      <c r="D33" t="s">
+        <v>635</v>
+      </c>
+      <c r="E33" t="s">
+        <v>636</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>638</v>
+      </c>
+      <c r="B34" t="s">
+        <v>639</v>
+      </c>
+      <c r="C34" t="s">
+        <v>640</v>
+      </c>
+      <c r="D34" t="s">
+        <v>641</v>
+      </c>
+      <c r="E34" t="s">
+        <v>642</v>
+      </c>
+      <c r="F34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>644</v>
+      </c>
+      <c r="B35" t="s">
+        <v>645</v>
+      </c>
+      <c r="C35" t="s">
+        <v>646</v>
+      </c>
+      <c r="D35" t="s">
+        <v>647</v>
+      </c>
+      <c r="E35" t="s">
+        <v>648</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>650</v>
+      </c>
+      <c r="B36" t="s">
+        <v>651</v>
+      </c>
+      <c r="C36" t="s">
+        <v>652</v>
+      </c>
+      <c r="D36" t="s">
+        <v>653</v>
+      </c>
+      <c r="E36" t="s">
+        <v>654</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>656</v>
+      </c>
+      <c r="B37" t="s">
+        <v>657</v>
+      </c>
+      <c r="C37" t="s">
+        <v>658</v>
+      </c>
+      <c r="D37" t="s">
+        <v>659</v>
+      </c>
+      <c r="E37" t="s">
+        <v>660</v>
+      </c>
+      <c r="F37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>662</v>
+      </c>
+      <c r="B38" t="s">
+        <v>663</v>
+      </c>
+      <c r="C38" t="s">
+        <v>664</v>
+      </c>
+      <c r="D38" t="s">
+        <v>665</v>
+      </c>
+      <c r="E38" t="s">
+        <v>666</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>668</v>
+      </c>
+      <c r="B39" t="s">
+        <v>669</v>
+      </c>
+      <c r="C39" t="s">
+        <v>589</v>
+      </c>
+      <c r="D39" t="s">
+        <v>670</v>
+      </c>
+      <c r="E39" t="s">
+        <v>671</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>673</v>
+      </c>
+      <c r="B40" t="s">
+        <v>674</v>
+      </c>
+      <c r="C40" t="s">
+        <v>675</v>
+      </c>
+      <c r="D40" t="s">
+        <v>676</v>
+      </c>
+      <c r="E40" t="s">
+        <v>677</v>
+      </c>
+      <c r="F40" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>678</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feature: lecture 4th added
</commit_message>
<xml_diff>
--- a/public/innovation_marketing_questions.xlsx
+++ b/public/innovation_marketing_questions.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrykostern/Documents/code/innovation-mgt/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6B0F3B-5A25-ED4B-98A3-2A33EA18A5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42EFC47-8253-9445-81E4-B1F53884A143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principles of Marketing &amp; Ethic" sheetId="1" r:id="rId1"/>
     <sheet name="Marketing Strategy and Environm" sheetId="2" r:id="rId2"/>
     <sheet name="Creating Customer Value, Satisf" sheetId="3" r:id="rId3"/>
+    <sheet name="Digital Marketing, Information " sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="913">
   <si>
     <t>Question</t>
   </si>
@@ -2065,6 +2066,702 @@
   </si>
   <si>
     <t>$p_{j,t}$ is the survival probability that the customer stays beyond period t.</t>
+  </si>
+  <si>
+    <t>A Marketing Information System (MIS) does not include which of the following components?</t>
+  </si>
+  <si>
+    <t>Equipment to collect data</t>
+  </si>
+  <si>
+    <t>Procedures to evaluate information</t>
+  </si>
+  <si>
+    <t>Methods to predict stock market fluctuations</t>
+  </si>
+  <si>
+    <t>People to distribute insights to decision makers</t>
+  </si>
+  <si>
+    <t>MIS focuses on marketing data gathering and distribution, not financial market forecasting.</t>
+  </si>
+  <si>
+    <t>Which source is considered an external input to an MIS?</t>
+  </si>
+  <si>
+    <t>Sales transaction records</t>
+  </si>
+  <si>
+    <t>Customer complaint logs</t>
+  </si>
+  <si>
+    <t>Syndicated market reports</t>
+  </si>
+  <si>
+    <t>Employee performance reviews</t>
+  </si>
+  <si>
+    <t>Syndicated reports come from outside the firm, unlike internal records.</t>
+  </si>
+  <si>
+    <t>“Big Data” in marketing primarily presents the challenge of:</t>
+  </si>
+  <si>
+    <t>Acquiring any data at all</t>
+  </si>
+  <si>
+    <t>Storing minimal datasets efficiently</t>
+  </si>
+  <si>
+    <t>Converting massive quantities into actionable insights</t>
+  </si>
+  <si>
+    <t>Ensuring no new information is collected</t>
+  </si>
+  <si>
+    <t>Marketers need better—rather than more—information and must process it effectively.</t>
+  </si>
+  <si>
+    <t>Which technology is not typically part of database marketing?</t>
+  </si>
+  <si>
+    <t>Data warehousing</t>
+  </si>
+  <si>
+    <t>Data mining</t>
+  </si>
+  <si>
+    <t>Customer relationship management</t>
+  </si>
+  <si>
+    <t>Virtual reality prototyping</t>
+  </si>
+  <si>
+    <t>VR prototyping is not a core database marketing tool.</t>
+  </si>
+  <si>
+    <t>Online behavioral tracking aims to:</t>
+  </si>
+  <si>
+    <t>Track social media conversations only</t>
+  </si>
+  <si>
+    <t>Target ads based on a customer’s Web behavior</t>
+  </si>
+  <si>
+    <t>Replace traditional CRM systems entirely</t>
+  </si>
+  <si>
+    <t>Eliminate the need for data mining</t>
+  </si>
+  <si>
+    <t>It uses browsing and purchase behavior to tailor marketing offers.</t>
+  </si>
+  <si>
+    <t>Social‐tracking targeting differs from behavioral tracking by focusing on:</t>
+  </si>
+  <si>
+    <t>Offline purchase data</t>
+  </si>
+  <si>
+    <t>Customers’ social network connections and conversations</t>
+  </si>
+  <si>
+    <t>Transactional CRM databases</t>
+  </si>
+  <si>
+    <t>Web server logs only</t>
+  </si>
+  <si>
+    <t>It leverages social interactions to inform targeting.</t>
+  </si>
+  <si>
+    <t>Market research is defined as the systematic design, collection, analysis, and reporting of data relevant to:</t>
+  </si>
+  <si>
+    <t>Any corporate decision</t>
+  </si>
+  <si>
+    <t>A specific marketing situation</t>
+  </si>
+  <si>
+    <t>Financial accounting standards</t>
+  </si>
+  <si>
+    <t>Human resources management</t>
+  </si>
+  <si>
+    <t>It addresses particular marketing challenges.</t>
+  </si>
+  <si>
+    <t>Which of these is not one of the six steps of the market research process?</t>
+  </si>
+  <si>
+    <t>Define the problem and research objectives</t>
+  </si>
+  <si>
+    <t>Develop the research plan</t>
+  </si>
+  <si>
+    <t>Increase product price arbitrarily</t>
+  </si>
+  <si>
+    <t>Make the decision</t>
+  </si>
+  <si>
+    <t>Pricing decisions follow, but are not a research step.</t>
+  </si>
+  <si>
+    <t>In the S–O–R model, the O stands for:</t>
+  </si>
+  <si>
+    <t>Organism (consumer)</t>
+  </si>
+  <si>
+    <t>Offering</t>
+  </si>
+  <si>
+    <t>Obligation</t>
+  </si>
+  <si>
+    <t>Organism refers to the consumer’s internal processing.</t>
+  </si>
+  <si>
+    <t>Which research design is best when you have no strong hypotheses and need exploratory insights?</t>
+  </si>
+  <si>
+    <t>Descriptive</t>
+  </si>
+  <si>
+    <t>Explicative</t>
+  </si>
+  <si>
+    <t>Exploratory</t>
+  </si>
+  <si>
+    <t>Causal</t>
+  </si>
+  <si>
+    <t>Exploratory designs (e.g., focus groups) uncover initial ideas.</t>
+  </si>
+  <si>
+    <t>An experiment with no randomization and conducted in the field is called a:</t>
+  </si>
+  <si>
+    <t>Laboratory experiment</t>
+  </si>
+  <si>
+    <t>Quasi‐experiment</t>
+  </si>
+  <si>
+    <t>Simulated test market</t>
+  </si>
+  <si>
+    <t>Pilot survey</t>
+  </si>
+  <si>
+    <t>Field quasi‐experiments lack random assignment.</t>
+  </si>
+  <si>
+    <t>Which is not a characteristic of quantitative research?</t>
+  </si>
+  <si>
+    <t>Objective separation of researcher and subject</t>
+  </si>
+  <si>
+    <t>Focus on cause‐effect relationships</t>
+  </si>
+  <si>
+    <t>Subjective interpretation of multiple simultaneous causes</t>
+  </si>
+  <si>
+    <t>Generalizability of findings</t>
+  </si>
+  <si>
+    <t>That is a hallmark of qualitative research.</t>
+  </si>
+  <si>
+    <t>Independent variables (IV) in experiments are also known as:</t>
+  </si>
+  <si>
+    <t>Effect variables</t>
+  </si>
+  <si>
+    <t>Extraneous variables</t>
+  </si>
+  <si>
+    <t>Cause variables</t>
+  </si>
+  <si>
+    <t>Response variables</t>
+  </si>
+  <si>
+    <t>IVs are the hypothesized causes.</t>
+  </si>
+  <si>
+    <t>Which survey construction rule should you follow?</t>
+  </si>
+  <si>
+    <t>Use double negatives for clarity</t>
+  </si>
+  <si>
+    <t>Employ sophisticated jargon to sound expert</t>
+  </si>
+  <si>
+    <t>Make questions specific and simple</t>
+  </si>
+  <si>
+    <t>Avoid ‘other’ options in fixed‐response items</t>
+  </si>
+  <si>
+    <t>Simplicity and specificity reduce bias.</t>
+  </si>
+  <si>
+    <t>A non‐probability sampling plan means:</t>
+  </si>
+  <si>
+    <t>Every population member has a known chance of selection</t>
+  </si>
+  <si>
+    <t>Selection is based on convenience or judgment</t>
+  </si>
+  <si>
+    <t>Randomized stratification is used</t>
+  </si>
+  <si>
+    <t>Sample size is always greater than 1,000</t>
+  </si>
+  <si>
+    <t>Non‐probability relies on subjective selection methods.</t>
+  </si>
+  <si>
+    <t>Which is not one of the “Do’s” of survey design in the lecture?</t>
+  </si>
+  <si>
+    <t>Avoid ambiguous words</t>
+  </si>
+  <si>
+    <t>Desensitize with response bands</t>
+  </si>
+  <si>
+    <t>Include hypotheticals freely</t>
+  </si>
+  <si>
+    <t>Allow an ‘other’ category</t>
+  </si>
+  <si>
+    <t>Hypothetical questions can confuse respondents.</t>
+  </si>
+  <si>
+    <t>A key characteristic of good market research is:</t>
+  </si>
+  <si>
+    <t>Exclusively using one method to save time</t>
+  </si>
+  <si>
+    <t>Healthy skepticism about data sources</t>
+  </si>
+  <si>
+    <t>Prioritizing speed over validity</t>
+  </si>
+  <si>
+    <t>Mixing research and promotional activities</t>
+  </si>
+  <si>
+    <t>Skepticism helps ensure data quality.</t>
+  </si>
+  <si>
+    <t>External marketing metrics include all except:</t>
+  </si>
+  <si>
+    <t>Market share</t>
+  </si>
+  <si>
+    <t>Employee satisfaction</t>
+  </si>
+  <si>
+    <t>Brand awareness</t>
+  </si>
+  <si>
+    <t>Customer complaints</t>
+  </si>
+  <si>
+    <t>Employee satisfaction is an internal metric.</t>
+  </si>
+  <si>
+    <t>Which metric belongs to internal metrics?</t>
+  </si>
+  <si>
+    <t>Relative price perception</t>
+  </si>
+  <si>
+    <t>Willingness to change</t>
+  </si>
+  <si>
+    <t>Behavioral loyalty</t>
+  </si>
+  <si>
+    <t>Perceived quality</t>
+  </si>
+  <si>
+    <t>Willingness to change reflects internal readiness.</t>
+  </si>
+  <si>
+    <t>Marketing‐mix modeling tools do not include:</t>
+  </si>
+  <si>
+    <t>Customer lifetime value analysis</t>
+  </si>
+  <si>
+    <t>Brand equity measures</t>
+  </si>
+  <si>
+    <t>Balanced scorecard</t>
+  </si>
+  <si>
+    <t>Social media posting schedules</t>
+  </si>
+  <si>
+    <t>Posting schedules are tactical, not modeling tools.</t>
+  </si>
+  <si>
+    <t>The balanced scorecard’s Learning and Growth perspective measures:</t>
+  </si>
+  <si>
+    <t>Financial ROI</t>
+  </si>
+  <si>
+    <t>Internal process efficiency</t>
+  </si>
+  <si>
+    <t>Employee skills and innovation support</t>
+  </si>
+  <si>
+    <t>Customer satisfaction</t>
+  </si>
+  <si>
+    <t>It tracks the organization’s capacity to improve.</t>
+  </si>
+  <si>
+    <t>The Declaration of German Market Researchers insists on:</t>
+  </si>
+  <si>
+    <t>Using only internal data sources</t>
+  </si>
+  <si>
+    <t>Integration of research with sales promotions</t>
+  </si>
+  <si>
+    <t>Anonymization and methodological objectivity</t>
+  </si>
+  <si>
+    <t>Ignoring reliability in favor of speed</t>
+  </si>
+  <si>
+    <t>It emphasizes ethics and objectivity.</t>
+  </si>
+  <si>
+    <t>Which is a qualitative data‐collection method?</t>
+  </si>
+  <si>
+    <t>Large‐scale online panel</t>
+  </si>
+  <si>
+    <t>Focus group discussions</t>
+  </si>
+  <si>
+    <t>Structured survey</t>
+  </si>
+  <si>
+    <t>Experiment with control group</t>
+  </si>
+  <si>
+    <t>Focus groups explore subjective experiences.</t>
+  </si>
+  <si>
+    <t>In explicative research designs, the primary goal is to:</t>
+  </si>
+  <si>
+    <t>Discover themes without prior hypotheses</t>
+  </si>
+  <si>
+    <t>Describe market characteristics</t>
+  </si>
+  <si>
+    <t>Test hypotheses about variable relationships</t>
+  </si>
+  <si>
+    <t>Collect purely secondary data</t>
+  </si>
+  <si>
+    <t>Explicative (causal) studies explain interrelationships.</t>
+  </si>
+  <si>
+    <t>A simulated test market experiment is typically conducted in:</t>
+  </si>
+  <si>
+    <t>A live retail environment</t>
+  </si>
+  <si>
+    <t>A controlled lab setting</t>
+  </si>
+  <si>
+    <t>Consumer homes with no control</t>
+  </si>
+  <si>
+    <t>Online surveys only</t>
+  </si>
+  <si>
+    <t>Labs replicate market conditions in a controlled environment.</t>
+  </si>
+  <si>
+    <t>Which is not true about syndicated‐service market research firms?</t>
+  </si>
+  <si>
+    <t>They sell the same data to multiple clients</t>
+  </si>
+  <si>
+    <t>They conduct customized single‐company projects</t>
+  </si>
+  <si>
+    <t>They typically track industry‐wide metrics</t>
+  </si>
+  <si>
+    <t>They provide ongoing data series</t>
+  </si>
+  <si>
+    <t>Custom single‐company studies are done by custom‐research firms.</t>
+  </si>
+  <si>
+    <t>Data mining in online environments allows marketers to:</t>
+  </si>
+  <si>
+    <t>Eliminate customer surveys</t>
+  </si>
+  <si>
+    <t>Identify hidden patterns in large datasets</t>
+  </si>
+  <si>
+    <t>Conduct only qualitative analysis</t>
+  </si>
+  <si>
+    <t>Replace the need for sampling plans</t>
+  </si>
+  <si>
+    <t>It discovers non‐obvious relationships in big data.</t>
+  </si>
+  <si>
+    <t>Which of these is an external benefit of effective information management?</t>
+  </si>
+  <si>
+    <t>Faster employee onboarding</t>
+  </si>
+  <si>
+    <t>More accurate market forecasts</t>
+  </si>
+  <si>
+    <t>Reduced IT infrastructure costs</t>
+  </si>
+  <si>
+    <t>Improved internal communication</t>
+  </si>
+  <si>
+    <t>External benefits affect decisions about markets and customers.</t>
+  </si>
+  <si>
+    <t>Self‐service technologies in marketing INFORMATION MANAGEMENT refer to:</t>
+  </si>
+  <si>
+    <t>Automated customer data analysis tools</t>
+  </si>
+  <si>
+    <t>Machines that prepare physical products automatically</t>
+  </si>
+  <si>
+    <t>Help desks for employee queries</t>
+  </si>
+  <si>
+    <t>Outsourced research agencies</t>
+  </si>
+  <si>
+    <t>They let marketers or customers access data without intermediaries.</t>
+  </si>
+  <si>
+    <t>Which component is not part of a Marketing Intelligence System?</t>
+  </si>
+  <si>
+    <t>Competitor activity monitoring</t>
+  </si>
+  <si>
+    <t>Environmental trend analysis</t>
+  </si>
+  <si>
+    <t>Internal transaction processing</t>
+  </si>
+  <si>
+    <t>Daily news scanning</t>
+  </si>
+  <si>
+    <t>MIS handles internal transactions, while MIS uses external intelligence.</t>
+  </si>
+  <si>
+    <t>Ethical marketing under GDPR requires anonymization to protect:</t>
+  </si>
+  <si>
+    <t>Intellectual property</t>
+  </si>
+  <si>
+    <t>Personal data of respondents</t>
+  </si>
+  <si>
+    <t>Corporate financial reports</t>
+  </si>
+  <si>
+    <t>Patent applications</t>
+  </si>
+  <si>
+    <t>GDPR focuses on personal data privacy.</t>
+  </si>
+  <si>
+    <t>Which is a don’t when writing survey questions?</t>
+  </si>
+  <si>
+    <t>Use mutually exclusive categories</t>
+  </si>
+  <si>
+    <t>Avoid negatives</t>
+  </si>
+  <si>
+    <t>Utilize ambiguous wording</t>
+  </si>
+  <si>
+    <t>Ambiguity leads to unreliable responses.</t>
+  </si>
+  <si>
+    <t>Pilot surveys and expert interviews are examples of:</t>
+  </si>
+  <si>
+    <t>Descriptive research methods</t>
+  </si>
+  <si>
+    <t>Exploratory research methods</t>
+  </si>
+  <si>
+    <t>Explicative research methods</t>
+  </si>
+  <si>
+    <t>Marketing‐mix modeling</t>
+  </si>
+  <si>
+    <t>They generate hypotheses in exploratory stages.</t>
+  </si>
+  <si>
+    <t>Which perspective of the balanced scorecard asks How do we look to our shareholders?</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Internal business processes</t>
+  </si>
+  <si>
+    <t>Learning and growth</t>
+  </si>
+  <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>The financial perspective focuses on shareholder results.</t>
+  </si>
+  <si>
+    <t>Anonymization in market research primarily serves to:</t>
+  </si>
+  <si>
+    <t>Increase sample size</t>
+  </si>
+  <si>
+    <t>Protect respondents’ privacy</t>
+  </si>
+  <si>
+    <t>Enhance data mining speed</t>
+  </si>
+  <si>
+    <t>Lower research costs</t>
+  </si>
+  <si>
+    <t>Removing identifiers ensures data confidentiality.</t>
+  </si>
+  <si>
+    <t>Which is not typically included in the research‐plan development step?</t>
+  </si>
+  <si>
+    <t>Choosing data‐collection methods</t>
+  </si>
+  <si>
+    <t>Designing sampling procedures</t>
+  </si>
+  <si>
+    <t>Defining the research problem</t>
+  </si>
+  <si>
+    <t>Selecting analysis techniques</t>
+  </si>
+  <si>
+    <t>Problem definition occurs in Step 1, not Step 2.</t>
+  </si>
+  <si>
+    <t>Field experiments differ from lab experiments by:</t>
+  </si>
+  <si>
+    <t>Having stricter control over variables</t>
+  </si>
+  <si>
+    <t>Being conducted in real‐world environments</t>
+  </si>
+  <si>
+    <t>Never using control groups</t>
+  </si>
+  <si>
+    <t>Always randomizing subjects</t>
+  </si>
+  <si>
+    <t>Field studies take place in actual market settings.</t>
+  </si>
+  <si>
+    <t>Which sampling contact method can introduce interviewer bias?</t>
+  </si>
+  <si>
+    <t>Online survey</t>
+  </si>
+  <si>
+    <t>Telephone interview</t>
+  </si>
+  <si>
+    <t>Email questionnaire</t>
+  </si>
+  <si>
+    <t>Automated kiosk survey</t>
+  </si>
+  <si>
+    <t>Interviewer tone or wording can influence responses.</t>
+  </si>
+  <si>
+    <t>Customer lifetime value calculations most directly rely on:</t>
+  </si>
+  <si>
+    <t>Daily web‐site hits</t>
+  </si>
+  <si>
+    <t>Net present value of future profits</t>
+  </si>
+  <si>
+    <t>Number of survey completions</t>
+  </si>
+  <si>
+    <t>Balanced scorecard metrics</t>
+  </si>
+  <si>
+    <t>CLV is the discounted value of predicted future contribution margins.</t>
   </si>
 </sst>
 </file>
@@ -4375,7 +5072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0184A555-D137-5947-81F3-BEB4CF021670}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -5307,4 +6004,939 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3F16FA-93EC-7B49-A314-5D77C5F135A6}">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>681</v>
+      </c>
+      <c r="B2" t="s">
+        <v>682</v>
+      </c>
+      <c r="C2" t="s">
+        <v>683</v>
+      </c>
+      <c r="D2" t="s">
+        <v>684</v>
+      </c>
+      <c r="E2" t="s">
+        <v>685</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>687</v>
+      </c>
+      <c r="B3" t="s">
+        <v>688</v>
+      </c>
+      <c r="C3" t="s">
+        <v>689</v>
+      </c>
+      <c r="D3" t="s">
+        <v>690</v>
+      </c>
+      <c r="E3" t="s">
+        <v>691</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>693</v>
+      </c>
+      <c r="B4" t="s">
+        <v>694</v>
+      </c>
+      <c r="C4" t="s">
+        <v>695</v>
+      </c>
+      <c r="D4" t="s">
+        <v>696</v>
+      </c>
+      <c r="E4" t="s">
+        <v>697</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>699</v>
+      </c>
+      <c r="B5" t="s">
+        <v>700</v>
+      </c>
+      <c r="C5" t="s">
+        <v>701</v>
+      </c>
+      <c r="D5" t="s">
+        <v>702</v>
+      </c>
+      <c r="E5" t="s">
+        <v>703</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>705</v>
+      </c>
+      <c r="B6" t="s">
+        <v>706</v>
+      </c>
+      <c r="C6" t="s">
+        <v>707</v>
+      </c>
+      <c r="D6" t="s">
+        <v>708</v>
+      </c>
+      <c r="E6" t="s">
+        <v>709</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>711</v>
+      </c>
+      <c r="B7" t="s">
+        <v>712</v>
+      </c>
+      <c r="C7" t="s">
+        <v>713</v>
+      </c>
+      <c r="D7" t="s">
+        <v>714</v>
+      </c>
+      <c r="E7" t="s">
+        <v>715</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>717</v>
+      </c>
+      <c r="B8" t="s">
+        <v>718</v>
+      </c>
+      <c r="C8" t="s">
+        <v>719</v>
+      </c>
+      <c r="D8" t="s">
+        <v>720</v>
+      </c>
+      <c r="E8" t="s">
+        <v>721</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>723</v>
+      </c>
+      <c r="B9" t="s">
+        <v>724</v>
+      </c>
+      <c r="C9" t="s">
+        <v>725</v>
+      </c>
+      <c r="D9" t="s">
+        <v>726</v>
+      </c>
+      <c r="E9" t="s">
+        <v>727</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>729</v>
+      </c>
+      <c r="B10" t="s">
+        <v>368</v>
+      </c>
+      <c r="C10" t="s">
+        <v>730</v>
+      </c>
+      <c r="D10" t="s">
+        <v>731</v>
+      </c>
+      <c r="E10" t="s">
+        <v>732</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>734</v>
+      </c>
+      <c r="B11" t="s">
+        <v>735</v>
+      </c>
+      <c r="C11" t="s">
+        <v>736</v>
+      </c>
+      <c r="D11" t="s">
+        <v>737</v>
+      </c>
+      <c r="E11" t="s">
+        <v>738</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>740</v>
+      </c>
+      <c r="B12" t="s">
+        <v>741</v>
+      </c>
+      <c r="C12" t="s">
+        <v>742</v>
+      </c>
+      <c r="D12" t="s">
+        <v>743</v>
+      </c>
+      <c r="E12" t="s">
+        <v>744</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>746</v>
+      </c>
+      <c r="B13" t="s">
+        <v>747</v>
+      </c>
+      <c r="C13" t="s">
+        <v>748</v>
+      </c>
+      <c r="D13" t="s">
+        <v>749</v>
+      </c>
+      <c r="E13" t="s">
+        <v>750</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>752</v>
+      </c>
+      <c r="B14" t="s">
+        <v>753</v>
+      </c>
+      <c r="C14" t="s">
+        <v>754</v>
+      </c>
+      <c r="D14" t="s">
+        <v>755</v>
+      </c>
+      <c r="E14" t="s">
+        <v>756</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>758</v>
+      </c>
+      <c r="B15" t="s">
+        <v>759</v>
+      </c>
+      <c r="C15" t="s">
+        <v>760</v>
+      </c>
+      <c r="D15" t="s">
+        <v>761</v>
+      </c>
+      <c r="E15" t="s">
+        <v>762</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>764</v>
+      </c>
+      <c r="B16" t="s">
+        <v>765</v>
+      </c>
+      <c r="C16" t="s">
+        <v>766</v>
+      </c>
+      <c r="D16" t="s">
+        <v>767</v>
+      </c>
+      <c r="E16" t="s">
+        <v>768</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>770</v>
+      </c>
+      <c r="B17" t="s">
+        <v>771</v>
+      </c>
+      <c r="C17" t="s">
+        <v>772</v>
+      </c>
+      <c r="D17" t="s">
+        <v>773</v>
+      </c>
+      <c r="E17" t="s">
+        <v>774</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>776</v>
+      </c>
+      <c r="B18" t="s">
+        <v>777</v>
+      </c>
+      <c r="C18" t="s">
+        <v>778</v>
+      </c>
+      <c r="D18" t="s">
+        <v>779</v>
+      </c>
+      <c r="E18" t="s">
+        <v>780</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>782</v>
+      </c>
+      <c r="B19" t="s">
+        <v>783</v>
+      </c>
+      <c r="C19" t="s">
+        <v>784</v>
+      </c>
+      <c r="D19" t="s">
+        <v>785</v>
+      </c>
+      <c r="E19" t="s">
+        <v>786</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>788</v>
+      </c>
+      <c r="B20" t="s">
+        <v>789</v>
+      </c>
+      <c r="C20" t="s">
+        <v>790</v>
+      </c>
+      <c r="D20" t="s">
+        <v>791</v>
+      </c>
+      <c r="E20" t="s">
+        <v>792</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>794</v>
+      </c>
+      <c r="B21" t="s">
+        <v>795</v>
+      </c>
+      <c r="C21" t="s">
+        <v>796</v>
+      </c>
+      <c r="D21" t="s">
+        <v>797</v>
+      </c>
+      <c r="E21" t="s">
+        <v>798</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>800</v>
+      </c>
+      <c r="B22" t="s">
+        <v>801</v>
+      </c>
+      <c r="C22" t="s">
+        <v>802</v>
+      </c>
+      <c r="D22" t="s">
+        <v>803</v>
+      </c>
+      <c r="E22" t="s">
+        <v>804</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>806</v>
+      </c>
+      <c r="B23" t="s">
+        <v>807</v>
+      </c>
+      <c r="C23" t="s">
+        <v>808</v>
+      </c>
+      <c r="D23" t="s">
+        <v>809</v>
+      </c>
+      <c r="E23" t="s">
+        <v>810</v>
+      </c>
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>812</v>
+      </c>
+      <c r="B24" t="s">
+        <v>813</v>
+      </c>
+      <c r="C24" t="s">
+        <v>814</v>
+      </c>
+      <c r="D24" t="s">
+        <v>815</v>
+      </c>
+      <c r="E24" t="s">
+        <v>816</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>818</v>
+      </c>
+      <c r="B25" t="s">
+        <v>819</v>
+      </c>
+      <c r="C25" t="s">
+        <v>820</v>
+      </c>
+      <c r="D25" t="s">
+        <v>821</v>
+      </c>
+      <c r="E25" t="s">
+        <v>822</v>
+      </c>
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>824</v>
+      </c>
+      <c r="B26" t="s">
+        <v>825</v>
+      </c>
+      <c r="C26" t="s">
+        <v>826</v>
+      </c>
+      <c r="D26" t="s">
+        <v>827</v>
+      </c>
+      <c r="E26" t="s">
+        <v>828</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>830</v>
+      </c>
+      <c r="B27" t="s">
+        <v>831</v>
+      </c>
+      <c r="C27" t="s">
+        <v>832</v>
+      </c>
+      <c r="D27" t="s">
+        <v>833</v>
+      </c>
+      <c r="E27" t="s">
+        <v>834</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>836</v>
+      </c>
+      <c r="B28" t="s">
+        <v>837</v>
+      </c>
+      <c r="C28" t="s">
+        <v>838</v>
+      </c>
+      <c r="D28" t="s">
+        <v>839</v>
+      </c>
+      <c r="E28" t="s">
+        <v>840</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>842</v>
+      </c>
+      <c r="B29" t="s">
+        <v>843</v>
+      </c>
+      <c r="C29" t="s">
+        <v>844</v>
+      </c>
+      <c r="D29" t="s">
+        <v>845</v>
+      </c>
+      <c r="E29" t="s">
+        <v>846</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>848</v>
+      </c>
+      <c r="B30" t="s">
+        <v>849</v>
+      </c>
+      <c r="C30" t="s">
+        <v>850</v>
+      </c>
+      <c r="D30" t="s">
+        <v>851</v>
+      </c>
+      <c r="E30" t="s">
+        <v>852</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>854</v>
+      </c>
+      <c r="B31" t="s">
+        <v>855</v>
+      </c>
+      <c r="C31" t="s">
+        <v>856</v>
+      </c>
+      <c r="D31" t="s">
+        <v>857</v>
+      </c>
+      <c r="E31" t="s">
+        <v>858</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>860</v>
+      </c>
+      <c r="B32" t="s">
+        <v>861</v>
+      </c>
+      <c r="C32" t="s">
+        <v>862</v>
+      </c>
+      <c r="D32" t="s">
+        <v>863</v>
+      </c>
+      <c r="E32" t="s">
+        <v>864</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>866</v>
+      </c>
+      <c r="B33" t="s">
+        <v>867</v>
+      </c>
+      <c r="C33" t="s">
+        <v>868</v>
+      </c>
+      <c r="D33" t="s">
+        <v>869</v>
+      </c>
+      <c r="E33" t="s">
+        <v>772</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>871</v>
+      </c>
+      <c r="B34" t="s">
+        <v>872</v>
+      </c>
+      <c r="C34" t="s">
+        <v>873</v>
+      </c>
+      <c r="D34" t="s">
+        <v>874</v>
+      </c>
+      <c r="E34" t="s">
+        <v>875</v>
+      </c>
+      <c r="F34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>877</v>
+      </c>
+      <c r="B35" t="s">
+        <v>878</v>
+      </c>
+      <c r="C35" t="s">
+        <v>879</v>
+      </c>
+      <c r="D35" t="s">
+        <v>880</v>
+      </c>
+      <c r="E35" t="s">
+        <v>881</v>
+      </c>
+      <c r="F35" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>883</v>
+      </c>
+      <c r="B36" t="s">
+        <v>884</v>
+      </c>
+      <c r="C36" t="s">
+        <v>885</v>
+      </c>
+      <c r="D36" t="s">
+        <v>886</v>
+      </c>
+      <c r="E36" t="s">
+        <v>887</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>889</v>
+      </c>
+      <c r="B37" t="s">
+        <v>890</v>
+      </c>
+      <c r="C37" t="s">
+        <v>891</v>
+      </c>
+      <c r="D37" t="s">
+        <v>892</v>
+      </c>
+      <c r="E37" t="s">
+        <v>893</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>895</v>
+      </c>
+      <c r="B38" t="s">
+        <v>896</v>
+      </c>
+      <c r="C38" t="s">
+        <v>897</v>
+      </c>
+      <c r="D38" t="s">
+        <v>898</v>
+      </c>
+      <c r="E38" t="s">
+        <v>899</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>901</v>
+      </c>
+      <c r="B39" t="s">
+        <v>902</v>
+      </c>
+      <c r="C39" t="s">
+        <v>903</v>
+      </c>
+      <c r="D39" t="s">
+        <v>904</v>
+      </c>
+      <c r="E39" t="s">
+        <v>905</v>
+      </c>
+      <c r="F39" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>907</v>
+      </c>
+      <c r="B40" t="s">
+        <v>908</v>
+      </c>
+      <c r="C40" t="s">
+        <v>909</v>
+      </c>
+      <c r="D40" t="s">
+        <v>910</v>
+      </c>
+      <c r="E40" t="s">
+        <v>911</v>
+      </c>
+      <c r="F40" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>912</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feature: add topic 5th
</commit_message>
<xml_diff>
--- a/public/innovation_marketing_questions.xlsx
+++ b/public/innovation_marketing_questions.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrykostern/Documents/code/innovation-mgt/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42EFC47-8253-9445-81E4-B1F53884A143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79761774-48E2-7942-9A21-8239879D72D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principles of Marketing &amp; Ethic" sheetId="1" r:id="rId1"/>
     <sheet name="Marketing Strategy and Environm" sheetId="2" r:id="rId2"/>
     <sheet name="Creating Customer Value, Satisf" sheetId="3" r:id="rId3"/>
     <sheet name="Digital Marketing, Information " sheetId="4" r:id="rId4"/>
+    <sheet name="Analysing Business and Consumer" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="1116">
   <si>
     <t>Question</t>
   </si>
@@ -2762,6 +2763,615 @@
   </si>
   <si>
     <t>CLV is the discounted value of predicted future contribution margins.</t>
+  </si>
+  <si>
+    <t>Which of the following is not a characteristic of B2B markets?</t>
+  </si>
+  <si>
+    <t>Few and large buyers</t>
+  </si>
+  <si>
+    <t>Many buying influences</t>
+  </si>
+  <si>
+    <t>Price-driven impulse purchases</t>
+  </si>
+  <si>
+    <t>Geographically concentrated buyers</t>
+  </si>
+  <si>
+    <t>B2B purchases are typically planned and complex, not impulse-driven.</t>
+  </si>
+  <si>
+    <t>In a buying center, the person who actually signs the purchase order is called the:</t>
+  </si>
+  <si>
+    <t>Influencer</t>
+  </si>
+  <si>
+    <t>Gatekeeper</t>
+  </si>
+  <si>
+    <t>Buyer</t>
+  </si>
+  <si>
+    <t>Decider</t>
+  </si>
+  <si>
+    <t>The Buyer executes the transaction; the Decider chooses the supplier.</t>
+  </si>
+  <si>
+    <t>Key Account Management focuses primarily on:</t>
+  </si>
+  <si>
+    <t>One-time large orders</t>
+  </si>
+  <si>
+    <t>Transactional selling</t>
+  </si>
+  <si>
+    <t>Long-term relationship building with high-value customers</t>
+  </si>
+  <si>
+    <t>Exclusive use of intermediaries</t>
+  </si>
+  <si>
+    <t>It aims for sustainable, high-CLV relationships.</t>
+  </si>
+  <si>
+    <t>Organizational buying refers to:</t>
+  </si>
+  <si>
+    <t>Households buying consumer goods</t>
+  </si>
+  <si>
+    <t>Firms establishing needs, evaluating, and selecting suppliers</t>
+  </si>
+  <si>
+    <t>Impulse buying in retail settings</t>
+  </si>
+  <si>
+    <t>Crowd-funded project contributions</t>
+  </si>
+  <si>
+    <t>It’s the formal process firms use to purchase products/services.</t>
+  </si>
+  <si>
+    <t>One lesson from the Berlin Airport (BER) case is the need for:</t>
+  </si>
+  <si>
+    <t>More competitive bidding rounds</t>
+  </si>
+  <si>
+    <t>Integrated project management and clear ownership</t>
+  </si>
+  <si>
+    <t>Decentralized communication channels</t>
+  </si>
+  <si>
+    <t>Minimizing stakeholder involvement</t>
+  </si>
+  <si>
+    <t>Misaligned incentives and unclear roles derailed the project.</t>
+  </si>
+  <si>
+    <t>In the S–O–R model of consumer behavior, “O” stands for:</t>
+  </si>
+  <si>
+    <t>Offer</t>
+  </si>
+  <si>
+    <t>Opportunity</t>
+  </si>
+  <si>
+    <t>It refers to the consumer’s internal processes.</t>
+  </si>
+  <si>
+    <t>Which level is not one of the three consumer characteristic levels?</t>
+  </si>
+  <si>
+    <t>Sensation differs from perception in that sensation is:</t>
+  </si>
+  <si>
+    <t>Interpretation of stimuli</t>
+  </si>
+  <si>
+    <t>Immediate receptor response to stimuli</t>
+  </si>
+  <si>
+    <t>Memory integration</t>
+  </si>
+  <si>
+    <t>Post-purchase evaluation</t>
+  </si>
+  <si>
+    <t>Sensation is the raw input; perception organizes and interprets it.</t>
+  </si>
+  <si>
+    <t>An example of multimodal advertising would combine:</t>
+  </si>
+  <si>
+    <t>Print ads only</t>
+  </si>
+  <si>
+    <t>Audio, visual, and haptic cues</t>
+  </si>
+  <si>
+    <t>Single-sense billboards</t>
+  </si>
+  <si>
+    <t>Text messages alone</t>
+  </si>
+  <si>
+    <t>Multimodal engages multiple senses simultaneously.</t>
+  </si>
+  <si>
+    <t>According to behavioral learning theory, in classical conditioning a(n):</t>
+  </si>
+  <si>
+    <t>Reward follows a desired behavior</t>
+  </si>
+  <si>
+    <t>Unconditioned stimulus is paired with a neutral stimulus</t>
+  </si>
+  <si>
+    <t>Customer surveys are administered</t>
+  </si>
+  <si>
+    <t>Price discounts condition repeat purchase</t>
+  </si>
+  <si>
+    <t>A neutral stimulus becomes conditioned via pairing.</t>
+  </si>
+  <si>
+    <t>Maslow’s hierarchy of needs places “self-actualization” at the:</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Second level</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>It’s the highest level of motivational needs.</t>
+  </si>
+  <si>
+    <t>Which type of advertising appeals directly to a physiological need?</t>
+  </si>
+  <si>
+    <t>Luxury car ads</t>
+  </si>
+  <si>
+    <t>Food product ads</t>
+  </si>
+  <si>
+    <t>Charity donation appeals</t>
+  </si>
+  <si>
+    <t>Investment service ads</t>
+  </si>
+  <si>
+    <t>Hunger is a physiological need.</t>
+  </si>
+  <si>
+    <t>Involvement in the buying process is defined as:</t>
+  </si>
+  <si>
+    <t>Frequency of purchase</t>
+  </si>
+  <si>
+    <t>Perceived relevance based on needs, values, and interests</t>
+  </si>
+  <si>
+    <t>Social proof usage</t>
+  </si>
+  <si>
+    <t>Visual appeal of packaging</t>
+  </si>
+  <si>
+    <t>Involvement rises with personal relevance.</t>
+  </si>
+  <si>
+    <t>Which step in the consumer decision-making process comes immediately after problem recognition?</t>
+  </si>
+  <si>
+    <t>Purchase decision</t>
+  </si>
+  <si>
+    <t>Information search</t>
+  </si>
+  <si>
+    <t>Post-purchase behavior</t>
+  </si>
+  <si>
+    <t>Evaluation of alternatives</t>
+  </si>
+  <si>
+    <t>Shoppers seek data once they see a need.</t>
+  </si>
+  <si>
+    <t>Consumers may use heuristics during evaluation to:</t>
+  </si>
+  <si>
+    <t>Analyze every attribute equally</t>
+  </si>
+  <si>
+    <t>Simplify complex choices with mental shortcuts</t>
+  </si>
+  <si>
+    <t>Ignore brand entirely</t>
+  </si>
+  <si>
+    <t>Always select the cheapest option</t>
+  </si>
+  <si>
+    <t>Efficiency under time pressure drives heuristic use.</t>
+  </si>
+  <si>
+    <t>The lexicographic heuristic chooses the option with:</t>
+  </si>
+  <si>
+    <t>Highest score on the single most important attribute</t>
+  </si>
+  <si>
+    <t>Average across all attributes</t>
+  </si>
+  <si>
+    <t>Worst score eliminated first</t>
+  </si>
+  <si>
+    <t>Random selection</t>
+  </si>
+  <si>
+    <t>Shoppers rank alternatives by key attribute.</t>
+  </si>
+  <si>
+    <t>Beliefs differ from attitudes in that beliefs are:</t>
+  </si>
+  <si>
+    <t>Emotional evaluations</t>
+  </si>
+  <si>
+    <t>Thoughts about product attributes</t>
+  </si>
+  <si>
+    <t>Behavioral intentions</t>
+  </si>
+  <si>
+    <t>Impulse reactions</t>
+  </si>
+  <si>
+    <t>Attitudes are favorable/unfavorable evaluations.</t>
+  </si>
+  <si>
+    <t>Which is not a type of perceived risk in purchase decisions?</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Aesthetic</t>
+  </si>
+  <si>
+    <t>Time-related</t>
+  </si>
+  <si>
+    <t>Aesthetic risk falls under psychological or functional.</t>
+  </si>
+  <si>
+    <t>Value co-creation post-purchase includes all except:</t>
+  </si>
+  <si>
+    <t>Supporting “in use” interactions</t>
+  </si>
+  <si>
+    <t>Encouraging network relationships</t>
+  </si>
+  <si>
+    <t>Complete elimination of customer support</t>
+  </si>
+  <si>
+    <t>Engaging employees and partners</t>
+  </si>
+  <si>
+    <t>Support is vital, not eliminated.</t>
+  </si>
+  <si>
+    <t>Cognitive dissonance after buying can be reduced by:</t>
+  </si>
+  <si>
+    <t>Ignoring customer feedback</t>
+  </si>
+  <si>
+    <t>Offering money-back guarantees</t>
+  </si>
+  <si>
+    <t>Removing all warranties</t>
+  </si>
+  <si>
+    <t>Raising price post-purchase</t>
+  </si>
+  <si>
+    <t>Guarantees reassure the buyer.</t>
+  </si>
+  <si>
+    <t>Sustainable consumption in postpurchase behavior emphasizes:</t>
+  </si>
+  <si>
+    <t>Single-use products</t>
+  </si>
+  <si>
+    <t>Long-term environmental and social value</t>
+  </si>
+  <si>
+    <t>Planned obsolescence</t>
+  </si>
+  <si>
+    <t>Exclusive cost focus</t>
+  </si>
+  <si>
+    <t>Sustainability integrates eco and social considerations.</t>
+  </si>
+  <si>
+    <t>Habitual and impulse buying are contrasted based on:</t>
+  </si>
+  <si>
+    <t>Price only</t>
+  </si>
+  <si>
+    <t>Involvement level</t>
+  </si>
+  <si>
+    <t>Distribution channel</t>
+  </si>
+  <si>
+    <t>Brand equity</t>
+  </si>
+  <si>
+    <t>Low involvement yields habitual/impulse choices.</t>
+  </si>
+  <si>
+    <t>Which source is not among the four information search types?</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Psychological</t>
+  </si>
+  <si>
+    <t>The four are personal, commercial, public, experiential.</t>
+  </si>
+  <si>
+    <t>Consumers select more familiar brands when situations are ambiguous due to:</t>
+  </si>
+  <si>
+    <t>High involvement</t>
+  </si>
+  <si>
+    <t>Cognitive shortcuts</t>
+  </si>
+  <si>
+    <t>Brand loyalty lock-in</t>
+  </si>
+  <si>
+    <t>Price sensitivity</t>
+  </si>
+  <si>
+    <t>Ambiguity triggers heuristic reliance.</t>
+  </si>
+  <si>
+    <t>In the expectancy-value model, total evaluation is computed by:</t>
+  </si>
+  <si>
+    <t>Summing raw attribute scores</t>
+  </si>
+  <si>
+    <t>Multiplying each belief by its importance and summing</t>
+  </si>
+  <si>
+    <t>Averaging costs only</t>
+  </si>
+  <si>
+    <t>Ranking alternatives randomly</t>
+  </si>
+  <si>
+    <t>Weighted sum of beliefs × importance.</t>
+  </si>
+  <si>
+    <t>Elimination-by-aspects heuristic works by:</t>
+  </si>
+  <si>
+    <t>Comparing only the best alternative</t>
+  </si>
+  <si>
+    <t>Removing options that fail on key attributes sequentially</t>
+  </si>
+  <si>
+    <t>Calculating net present value</t>
+  </si>
+  <si>
+    <t>Using group consensus only</t>
+  </si>
+  <si>
+    <t>Options lacking minimum attribute levels are dropped.</t>
+  </si>
+  <si>
+    <t>The ABC model of attitude formation stands for:</t>
+  </si>
+  <si>
+    <t>Affect, Behavior, Cognition</t>
+  </si>
+  <si>
+    <t>Appeal, Brand, Choice</t>
+  </si>
+  <si>
+    <t>Awareness, Benefit, Cost</t>
+  </si>
+  <si>
+    <t>Acquisition, Belief, Compliance</t>
+  </si>
+  <si>
+    <t>It maps feelings, actions, and thoughts.</t>
+  </si>
+  <si>
+    <t>Which factor does not influence postpurchase value co-creation?</t>
+  </si>
+  <si>
+    <t>Network interactions</t>
+  </si>
+  <si>
+    <t>In-use support</t>
+  </si>
+  <si>
+    <t>Employee engagement</t>
+  </si>
+  <si>
+    <t>Up-front price only</t>
+  </si>
+  <si>
+    <t>Price impacts purchase, not co-creation.</t>
+  </si>
+  <si>
+    <t>Physical evidence in S–O–R includes all except:</t>
+  </si>
+  <si>
+    <t>Store layout</t>
+  </si>
+  <si>
+    <t>Packaging design</t>
+  </si>
+  <si>
+    <t>Employee uniforms</t>
+  </si>
+  <si>
+    <t>Consumer motivation</t>
+  </si>
+  <si>
+    <t>Motivation is part of “Organism”.</t>
+  </si>
+  <si>
+    <t>Under high involvement, consumers are more likely to:</t>
+  </si>
+  <si>
+    <t>Use heuristics exclusively</t>
+  </si>
+  <si>
+    <t>Engage in extensive information processing</t>
+  </si>
+  <si>
+    <t>Act on impulse only</t>
+  </si>
+  <si>
+    <t>Ignore product attributes</t>
+  </si>
+  <si>
+    <t>High involvement demands deeper evaluation.</t>
+  </si>
+  <si>
+    <t>Which step of the decision process can lead to word-of-mouth or complaints?</t>
+  </si>
+  <si>
+    <t>Postpurchase behavior</t>
+  </si>
+  <si>
+    <t>After buying, consumers share feedback.</t>
+  </si>
+  <si>
+    <t>Which is not an “Example from Multimodal Advertising”?</t>
+  </si>
+  <si>
+    <t>Scent-infused billboards</t>
+  </si>
+  <si>
+    <t>Interactive touch-screens</t>
+  </si>
+  <si>
+    <t>Plain text flyers</t>
+  </si>
+  <si>
+    <t>Audio-visual kiosks</t>
+  </si>
+  <si>
+    <t>Plain text engages only vision.</t>
+  </si>
+  <si>
+    <t>Motivation in consumer behavior is influenced by:</t>
+  </si>
+  <si>
+    <t>Sensation only</t>
+  </si>
+  <si>
+    <t>Needs and goals</t>
+  </si>
+  <si>
+    <t>Pricing solely</t>
+  </si>
+  <si>
+    <t>Package color exclusively</t>
+  </si>
+  <si>
+    <t>It stems from unmet needs and desired ends.</t>
+  </si>
+  <si>
+    <t>The first consumer decision step—problem recognition—occurs when:</t>
+  </si>
+  <si>
+    <t>A need arises from a discrepancy between actual and ideal state</t>
+  </si>
+  <si>
+    <t>The buyer completes post-purchase evaluation</t>
+  </si>
+  <si>
+    <t>The buyer finalizes payment method</t>
+  </si>
+  <si>
+    <t>A value co-creation opportunity appears</t>
+  </si>
+  <si>
+    <t>Recognition of a gap triggers the process.</t>
+  </si>
+  <si>
+    <t>Which is an external stimulus triggering problem recognition?</t>
+  </si>
+  <si>
+    <t>Boredom</t>
+  </si>
+  <si>
+    <t>A friend’s recommendation</t>
+  </si>
+  <si>
+    <t>Hunger pangs</t>
+  </si>
+  <si>
+    <t>Personal goals</t>
+  </si>
+  <si>
+    <t>External cues come from the environment.</t>
+  </si>
+  <si>
+    <t>Cultural</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>Political</t>
+  </si>
+  <si>
+    <t>The three are cultural, social and personal.</t>
   </si>
 </sst>
 </file>
@@ -6010,7 +6620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3F16FA-93EC-7B49-A314-5D77C5F135A6}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
@@ -6939,4 +7549,847 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6210F7E-A816-FD41-B9EF-4099C44BD41E}">
+  <dimension ref="A1:G36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>913</v>
+      </c>
+      <c r="B2" t="s">
+        <v>914</v>
+      </c>
+      <c r="C2" t="s">
+        <v>915</v>
+      </c>
+      <c r="D2" t="s">
+        <v>916</v>
+      </c>
+      <c r="E2" t="s">
+        <v>917</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>919</v>
+      </c>
+      <c r="B3" t="s">
+        <v>920</v>
+      </c>
+      <c r="C3" t="s">
+        <v>921</v>
+      </c>
+      <c r="D3" t="s">
+        <v>922</v>
+      </c>
+      <c r="E3" t="s">
+        <v>923</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>925</v>
+      </c>
+      <c r="B4" t="s">
+        <v>926</v>
+      </c>
+      <c r="C4" t="s">
+        <v>927</v>
+      </c>
+      <c r="D4" t="s">
+        <v>928</v>
+      </c>
+      <c r="E4" t="s">
+        <v>929</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>931</v>
+      </c>
+      <c r="B5" t="s">
+        <v>932</v>
+      </c>
+      <c r="C5" t="s">
+        <v>933</v>
+      </c>
+      <c r="D5" t="s">
+        <v>934</v>
+      </c>
+      <c r="E5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>937</v>
+      </c>
+      <c r="B6" t="s">
+        <v>938</v>
+      </c>
+      <c r="C6" t="s">
+        <v>939</v>
+      </c>
+      <c r="D6" t="s">
+        <v>940</v>
+      </c>
+      <c r="E6" t="s">
+        <v>941</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>943</v>
+      </c>
+      <c r="B7" t="s">
+        <v>944</v>
+      </c>
+      <c r="C7" t="s">
+        <v>730</v>
+      </c>
+      <c r="D7" t="s">
+        <v>945</v>
+      </c>
+      <c r="E7" t="s">
+        <v>305</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>947</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1114</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>948</v>
+      </c>
+      <c r="B9" t="s">
+        <v>949</v>
+      </c>
+      <c r="C9" t="s">
+        <v>950</v>
+      </c>
+      <c r="D9" t="s">
+        <v>951</v>
+      </c>
+      <c r="E9" t="s">
+        <v>952</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>954</v>
+      </c>
+      <c r="B10" t="s">
+        <v>955</v>
+      </c>
+      <c r="C10" t="s">
+        <v>956</v>
+      </c>
+      <c r="D10" t="s">
+        <v>957</v>
+      </c>
+      <c r="E10" t="s">
+        <v>958</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>960</v>
+      </c>
+      <c r="B11" t="s">
+        <v>961</v>
+      </c>
+      <c r="C11" t="s">
+        <v>962</v>
+      </c>
+      <c r="D11" t="s">
+        <v>963</v>
+      </c>
+      <c r="E11" t="s">
+        <v>964</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>966</v>
+      </c>
+      <c r="B12" t="s">
+        <v>967</v>
+      </c>
+      <c r="C12" t="s">
+        <v>968</v>
+      </c>
+      <c r="D12" t="s">
+        <v>969</v>
+      </c>
+      <c r="E12" t="s">
+        <v>970</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>972</v>
+      </c>
+      <c r="B13" t="s">
+        <v>973</v>
+      </c>
+      <c r="C13" t="s">
+        <v>974</v>
+      </c>
+      <c r="D13" t="s">
+        <v>975</v>
+      </c>
+      <c r="E13" t="s">
+        <v>976</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>978</v>
+      </c>
+      <c r="B14" t="s">
+        <v>979</v>
+      </c>
+      <c r="C14" t="s">
+        <v>980</v>
+      </c>
+      <c r="D14" t="s">
+        <v>981</v>
+      </c>
+      <c r="E14" t="s">
+        <v>982</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>984</v>
+      </c>
+      <c r="B15" t="s">
+        <v>985</v>
+      </c>
+      <c r="C15" t="s">
+        <v>986</v>
+      </c>
+      <c r="D15" t="s">
+        <v>987</v>
+      </c>
+      <c r="E15" t="s">
+        <v>988</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>990</v>
+      </c>
+      <c r="B16" t="s">
+        <v>991</v>
+      </c>
+      <c r="C16" t="s">
+        <v>992</v>
+      </c>
+      <c r="D16" t="s">
+        <v>993</v>
+      </c>
+      <c r="E16" t="s">
+        <v>994</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>996</v>
+      </c>
+      <c r="B17" t="s">
+        <v>997</v>
+      </c>
+      <c r="C17" t="s">
+        <v>998</v>
+      </c>
+      <c r="D17" t="s">
+        <v>999</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D19" t="s">
+        <v>881</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1017</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1029</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1083</v>
+      </c>
+      <c r="F31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B32" t="s">
+        <v>988</v>
+      </c>
+      <c r="C32" t="s">
+        <v>985</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E32" t="s">
+        <v>986</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1104</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1110</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feature: topic 8th done
</commit_message>
<xml_diff>
--- a/public/innovation_marketing_questions.xlsx
+++ b/public/innovation_marketing_questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrykostern/Documents/code/innovation-mgt/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BFAA39-B8F0-5548-B07B-1F76159D976E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96A332A-DF08-6148-BB48-F757D4EF0540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principles of Marketing &amp; Ethic" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,15 @@
     <sheet name="Analysing Business and Consumer" sheetId="5" r:id="rId5"/>
     <sheet name="Competition and Differentiation" sheetId="6" r:id="rId6"/>
     <sheet name="Segmenting, Targeting, and Posi" sheetId="7" r:id="rId7"/>
+    <sheet name="Products, Services and Brand Ma" sheetId="8" r:id="rId8"/>
+    <sheet name="Pricing" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="1560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="1751">
   <si>
     <t>Question</t>
   </si>
@@ -4706,6 +4708,579 @@
   </si>
   <si>
     <t>Create unique mental image in the customer’s mind</t>
+  </si>
+  <si>
+    <t>Which product life cycle pattern is characterized by repeated periods of decline and revival?</t>
+  </si>
+  <si>
+    <t>Scalloped</t>
+  </si>
+  <si>
+    <t>Fashion</t>
+  </si>
+  <si>
+    <t>Cycle-recycle</t>
+  </si>
+  <si>
+    <t>Growth-slump-maturity</t>
+  </si>
+  <si>
+    <t>The scalloped PLC features successive curves as new product variations revive sales.</t>
+  </si>
+  <si>
+    <t>A fad product life cycle differs from a fashion life cycle by having:</t>
+  </si>
+  <si>
+    <t>Multiple revivals over time</t>
+  </si>
+  <si>
+    <t>A very short rise and decline</t>
+  </si>
+  <si>
+    <t>Steady long-term growth</t>
+  </si>
+  <si>
+    <t>No decline phase</t>
+  </si>
+  <si>
+    <t>Fads have rapid adoption and decline, unlike fashions which cycle back.</t>
+  </si>
+  <si>
+    <t>In brand equity measurement, diagnosis focuses on:</t>
+  </si>
+  <si>
+    <t>Valuing the company for sale</t>
+  </si>
+  <si>
+    <t>Testing marketing mix impact on brand equity</t>
+  </si>
+  <si>
+    <t>Setting pricing strategy</t>
+  </si>
+  <si>
+    <t>Determining distribution channels</t>
+  </si>
+  <si>
+    <t>Diagnosis assesses how marketing actions affect brand equity levels.</t>
+  </si>
+  <si>
+    <t>Which of these is NOT a form of brand that can be legally protected?</t>
+  </si>
+  <si>
+    <t>Scent brands</t>
+  </si>
+  <si>
+    <t>Three-dimensional forms</t>
+  </si>
+  <si>
+    <t>Customer testimonials</t>
+  </si>
+  <si>
+    <t>Auditory brands</t>
+  </si>
+  <si>
+    <t>Testimonials are user-generated and not protectable as brand assets.</t>
+  </si>
+  <si>
+    <t>Interbrand’s annual ranking focuses on:</t>
+  </si>
+  <si>
+    <t>Number of trademarks filed</t>
+  </si>
+  <si>
+    <t>Brand financial performance and role in purchase decisions</t>
+  </si>
+  <si>
+    <t>Patent portfolios</t>
+  </si>
+  <si>
+    <t>Market share only</t>
+  </si>
+  <si>
+    <t>Interbrand values brands based on financial metrics and consumer perception.</t>
+  </si>
+  <si>
+    <t>A ‘branded house’ architecture implies:</t>
+  </si>
+  <si>
+    <t>Independent branding of each product</t>
+  </si>
+  <si>
+    <t>All products share the corporate brand name</t>
+  </si>
+  <si>
+    <t>No corporate brand presence</t>
+  </si>
+  <si>
+    <t>Only sub-brands matter</t>
+  </si>
+  <si>
+    <t>In a branded house, the master brand endorses all offerings.</t>
+  </si>
+  <si>
+    <t>Which diversification type involves entering a completely unrelated industry?</t>
+  </si>
+  <si>
+    <t>Horizontal</t>
+  </si>
+  <si>
+    <t>Vertical</t>
+  </si>
+  <si>
+    <t>Lateral</t>
+  </si>
+  <si>
+    <t>Concentric</t>
+  </si>
+  <si>
+    <t>Lateral diversification has no technological or commercial synergy with existing lines.</t>
+  </si>
+  <si>
+    <t>During the introduction stage of the product life cycle, firms should primarily focus on:</t>
+  </si>
+  <si>
+    <t>Maximizing profit</t>
+  </si>
+  <si>
+    <t>Building awareness</t>
+  </si>
+  <si>
+    <t>Harvesting cash flows</t>
+  </si>
+  <si>
+    <t>Extending line extensions</t>
+  </si>
+  <si>
+    <t>Introduction stage priorities are awareness and trial generation.</t>
+  </si>
+  <si>
+    <t>Which brand architecture strategy allows separate positioning and risk containment for each sub-brand?</t>
+  </si>
+  <si>
+    <t>House of brands</t>
+  </si>
+  <si>
+    <t>Branded house</t>
+  </si>
+  <si>
+    <t>Umbrella brand</t>
+  </si>
+  <si>
+    <t>Monolithic brand</t>
+  </si>
+  <si>
+    <t>A house of brands treats each brand independently, isolating risk.</t>
+  </si>
+  <si>
+    <t>The Technology Adoption Model posits that usage intention is driven by perceived usefulness and:</t>
+  </si>
+  <si>
+    <t>Brand loyalty</t>
+  </si>
+  <si>
+    <t>Perceived ease of use</t>
+  </si>
+  <si>
+    <t>Social proof</t>
+  </si>
+  <si>
+    <t>Perceived ease of use affects attitude toward using new technology.</t>
+  </si>
+  <si>
+    <t>Which adoption category includes individuals who adopt an offering soon after it's introduced?</t>
+  </si>
+  <si>
+    <t>Late majority</t>
+  </si>
+  <si>
+    <t>Early adopters</t>
+  </si>
+  <si>
+    <t>Laggards</t>
+  </si>
+  <si>
+    <t>Innovators</t>
+  </si>
+  <si>
+    <t>Early adopters follow innovators and help diffuse offerings.</t>
+  </si>
+  <si>
+    <t>A line extension is best described as:</t>
+  </si>
+  <si>
+    <t>Applying a brand to a new category</t>
+  </si>
+  <si>
+    <t>Introducing variation within the same product category</t>
+  </si>
+  <si>
+    <t>Dropping an existing offering</t>
+  </si>
+  <si>
+    <t>Merging two existing brands</t>
+  </si>
+  <si>
+    <t>Line extensions add flavors, sizes, or styles under the same brand.</t>
+  </si>
+  <si>
+    <t>Brand dilution risk increases when:</t>
+  </si>
+  <si>
+    <t>Extensions align with core brand associations</t>
+  </si>
+  <si>
+    <t>Too many unrelated extensions are introduced</t>
+  </si>
+  <si>
+    <t>Extensions share equity with the parent brand</t>
+  </si>
+  <si>
+    <t>Extensions improve overall brand visibility</t>
+  </si>
+  <si>
+    <t>Irrelevant extensions can erode brand meaning and equity.</t>
+  </si>
+  <si>
+    <t>Which of these is a key consequence of strong brand equity?</t>
+  </si>
+  <si>
+    <t>Lower consumer loyalty</t>
+  </si>
+  <si>
+    <t>Greater resilience to crises</t>
+  </si>
+  <si>
+    <t>Reduced perceived quality</t>
+  </si>
+  <si>
+    <t>Strong brands are less vulnerable to negative events.</t>
+  </si>
+  <si>
+    <t>Co-branding can achieve all EXCEPT:</t>
+  </si>
+  <si>
+    <t>Extended market reach</t>
+  </si>
+  <si>
+    <t>Shared development costs</t>
+  </si>
+  <si>
+    <t>Guaranteed brand equity enhancement</t>
+  </si>
+  <si>
+    <t>New consumer trial</t>
+  </si>
+  <si>
+    <t>Co-branding can fail and hurt partner equity if mismatches occur.</t>
+  </si>
+  <si>
+    <t>In the adoption process, the evaluation stage is when consumers:</t>
+  </si>
+  <si>
+    <t>Purchase the offering</t>
+  </si>
+  <si>
+    <t>Assess the product’s benefits and drawbacks</t>
+  </si>
+  <si>
+    <t>Become aware of the offering</t>
+  </si>
+  <si>
+    <t>Regularly repurchase</t>
+  </si>
+  <si>
+    <t>Evaluation involves mental or physical assessment before trial.</t>
+  </si>
+  <si>
+    <t>Which PLC pattern shows repeated growth troughs due to new feature introductions?</t>
+  </si>
+  <si>
+    <t>Cycle-recycle pattern features periodic resurgence aligned with marketing efforts.</t>
+  </si>
+  <si>
+    <t>Brand architecture decisions impact:</t>
+  </si>
+  <si>
+    <t>Only visual identity</t>
+  </si>
+  <si>
+    <t>Customer perception and managerial complexity</t>
+  </si>
+  <si>
+    <t>Patent registrations</t>
+  </si>
+  <si>
+    <t>Product quality exclusively</t>
+  </si>
+  <si>
+    <t>Architecture shapes how brands are perceived and managed.</t>
+  </si>
+  <si>
+    <t>A vertical diversification strategy might involve:</t>
+  </si>
+  <si>
+    <t>Launching a new unrelated consumer electronics line</t>
+  </si>
+  <si>
+    <t>Starting in-house manufacturing previously outsourced</t>
+  </si>
+  <si>
+    <t>Introducing a new flavor in the same product line</t>
+  </si>
+  <si>
+    <t>Extending brand to a new geographic region</t>
+  </si>
+  <si>
+    <t>Vertical diversification changes stage in supply chain, like backward integration.</t>
+  </si>
+  <si>
+    <t>Brand functions include all EXCEPT:</t>
+  </si>
+  <si>
+    <t>Offering legal protection</t>
+  </si>
+  <si>
+    <t>Signifying quality</t>
+  </si>
+  <si>
+    <t>Automating production processes</t>
+  </si>
+  <si>
+    <t>Creating growth opportunities</t>
+  </si>
+  <si>
+    <t>Brands do not directly automate production.</t>
+  </si>
+  <si>
+    <t>Which stakeholder perception contributes to brand knowledge?</t>
+  </si>
+  <si>
+    <t>Only financial analysts’ opinions</t>
+  </si>
+  <si>
+    <t>Consumers’ beliefs, images, feelings, and experiences</t>
+  </si>
+  <si>
+    <t>Supplier cost structures</t>
+  </si>
+  <si>
+    <t>Regulatory filings</t>
+  </si>
+  <si>
+    <t>Brand knowledge comprises consumer mental associations.</t>
+  </si>
+  <si>
+    <t>During maturity stage, product life cycle strategy often focuses on:</t>
+  </si>
+  <si>
+    <t>Driving trial among early adopters</t>
+  </si>
+  <si>
+    <t>Defending market share and extending product lines</t>
+  </si>
+  <si>
+    <t>Building initial awareness</t>
+  </si>
+  <si>
+    <t>Harvesting cash with minimal investment</t>
+  </si>
+  <si>
+    <t>Maturity requires differentiation and market segmentation.</t>
+  </si>
+  <si>
+    <t>The diagnostic use of brand equity helps managers:</t>
+  </si>
+  <si>
+    <t>Set tariffs on imports</t>
+  </si>
+  <si>
+    <t>Test whether marketing programs enhance brand strength</t>
+  </si>
+  <si>
+    <t>Decide employee salaries</t>
+  </si>
+  <si>
+    <t>Choose supplier contracts</t>
+  </si>
+  <si>
+    <t>Diagnosis measures program effects on brand health.</t>
+  </si>
+  <si>
+    <t>A radical new offering differs from incremental by:</t>
+  </si>
+  <si>
+    <t>Addressing similar needs with minor tweaks</t>
+  </si>
+  <si>
+    <t>Introducing a fundamentally novel technology or concept</t>
+  </si>
+  <si>
+    <t>Being solely a line extension</t>
+  </si>
+  <si>
+    <t>Sharing the same production process</t>
+  </si>
+  <si>
+    <t>Radical innovations break with existing designs or markets.</t>
+  </si>
+  <si>
+    <t>Elimination of offerings in a portfolio is undertaken to:</t>
+  </si>
+  <si>
+    <t>Increase brand dilution</t>
+  </si>
+  <si>
+    <t>Manage resource allocation and maintain focus</t>
+  </si>
+  <si>
+    <t>Maximize SKU proliferation</t>
+  </si>
+  <si>
+    <t>Prevent new product development</t>
+  </si>
+  <si>
+    <t>Dropping underperformers helps concentrate investments.</t>
+  </si>
+  <si>
+    <t>Which is NOT part of the consumer adoption concept stages?</t>
+  </si>
+  <si>
+    <t>Awareness</t>
+  </si>
+  <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>Trial</t>
+  </si>
+  <si>
+    <t>Integration is not a standard adoption stage.</t>
+  </si>
+  <si>
+    <t>A family brand architecture groups products by:</t>
+  </si>
+  <si>
+    <t>Separate unique names</t>
+  </si>
+  <si>
+    <t>Sub-brands under a category-specific umbrella</t>
+  </si>
+  <si>
+    <t>No naming convention</t>
+  </si>
+  <si>
+    <t>Random allocation</t>
+  </si>
+  <si>
+    <t>Family brands use a common name for a product line within a category.</t>
+  </si>
+  <si>
+    <t>Brand equity evaluation can support:</t>
+  </si>
+  <si>
+    <t>Licensing negotiations and valuation</t>
+  </si>
+  <si>
+    <t>Daily operational scheduling</t>
+  </si>
+  <si>
+    <t>Raw material sourcing</t>
+  </si>
+  <si>
+    <t>Evaluation provides arguments for licensing fees or brand sales.</t>
+  </si>
+  <si>
+    <t>A style PLC pattern exhibits:</t>
+  </si>
+  <si>
+    <t>A short-lived spike then decline</t>
+  </si>
+  <si>
+    <t>Cycle with periodic resurgence over decades</t>
+  </si>
+  <si>
+    <t>Permanent growth</t>
+  </si>
+  <si>
+    <t>Immediate collapse post-introduction</t>
+  </si>
+  <si>
+    <t>Styles maintain popularity over long periods with recurring interest.</t>
+  </si>
+  <si>
+    <t>Which is a disadvantage of category extensions?</t>
+  </si>
+  <si>
+    <t>Reduced development costs</t>
+  </si>
+  <si>
+    <t>Increased marketing efficiencies</t>
+  </si>
+  <si>
+    <t>Potential confusion and dilution of parent brand</t>
+  </si>
+  <si>
+    <t>Higher retailer acceptance</t>
+  </si>
+  <si>
+    <t>Entering new categories can confuse consumers about brand focus.</t>
+  </si>
+  <si>
+    <t>Incremental innovation is important because it:</t>
+  </si>
+  <si>
+    <t>Typically requires no marketing</t>
+  </si>
+  <si>
+    <t>Enhances existing offerings to sustain competitiveness</t>
+  </si>
+  <si>
+    <t>Always cannibalizes the core product</t>
+  </si>
+  <si>
+    <t>Prevents any brand extension</t>
+  </si>
+  <si>
+    <t>Incremental changes keep products relevant over time.</t>
+  </si>
+  <si>
+    <t>Which product portfolio change influences brand equity negatively if mishandled?</t>
+  </si>
+  <si>
+    <t>Strategic addition of new offerings</t>
+  </si>
+  <si>
+    <t>Brand extension aligned with core associations</t>
+  </si>
+  <si>
+    <t>Excessive and irrelevant extensions</t>
+  </si>
+  <si>
+    <t>Managed elimination of low-performers</t>
+  </si>
+  <si>
+    <t>Too many irrelevant extensions can dilute brand strength.</t>
+  </si>
+  <si>
+    <t>In a dual brand strategy, consumers might see:</t>
+  </si>
+  <si>
+    <t>Only the corporate name</t>
+  </si>
+  <si>
+    <t>No brand identity</t>
+  </si>
+  <si>
+    <t>Both the master brand and sub-brand names</t>
+  </si>
+  <si>
+    <t>Completely separate identities</t>
+  </si>
+  <si>
+    <t>Dual branding features corporate endorsement alongside product brands.</t>
   </si>
 </sst>
 </file>
@@ -10621,7 +11196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2DD5B2-14BF-C84D-88E2-C27FD2504A67}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -11573,4 +12148,813 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA45993-FB1B-504E-A0FA-0AAC69F3B04C}">
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1563</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1570</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1575</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1576</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1580</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1581</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1582</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1587</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1588</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1591</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1592</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1593</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1594</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1598</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1600</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1604</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1605</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1606</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1610</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1612</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1616</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1617</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1620</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1621</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1622</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1623</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1626</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1627</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1628</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1629</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1631</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1632</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1633</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1635</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1637</v>
+      </c>
+      <c r="B15" t="s">
+        <v>513</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1638</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1639</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1640</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1643</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1644</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1645</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1646</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1649</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1651</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1652</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B18" t="s">
+        <v>328</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1563</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1562</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1657</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1659</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1660</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1665</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1666</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1669</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1670</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1671</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1672</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1682</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1683</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1684</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1690</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1694</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1695</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1696</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1700</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1702</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1706</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1707</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1708</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1711</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1712</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1714</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B29" t="s">
+        <v>691</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1717</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1718</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1723</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1724</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1725</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1729</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1730</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1731</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1735</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1736</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1737</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1741</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1742</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1748</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1749</v>
+      </c>
+      <c r="F34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D105985-FAB0-684A-AE4B-535B19D8A727}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>